<commit_message>
Fix AwesomeImporter bug that appeared when running against azure
</commit_message>
<xml_diff>
--- a/TickListImporter.Test/Resources/AwesomeTickList.xlsx
+++ b/TickListImporter.Test/Resources/AwesomeTickList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="75" windowWidth="19320" windowHeight="7995"/>
+    <workbookView xWindow="2100" yWindow="75" windowWidth="19320" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <t>Grade</t>
   </si>
   <si>
-    <t>DateSet</t>
+    <t>Set</t>
   </si>
 </sst>
 </file>
@@ -3077,8 +3077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="G187" sqref="G187"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3132,9 +3132,9 @@
         <f>IF('[1]Complete Route Listing'!C10=0," ",'[1]Complete Route Listing'!C10)</f>
         <v>red</v>
       </c>
-      <c r="C2" s="7">
-        <f>IF('[1]Complete Route Listing'!D14=0," ",'[1]Complete Route Listing'!D14)</f>
-        <v>3</v>
+      <c r="C2" s="7" t="str">
+        <f>IF('[1]Complete Route Listing'!D10=0," ",'[1]Complete Route Listing'!D10)</f>
+        <v>3+</v>
       </c>
       <c r="D2" s="8" t="str">
         <f>IF('[1]Complete Route Listing'!F10=0," ",'[1]Complete Route Listing'!F10)</f>
@@ -3149,9 +3149,9 @@
         <f>IF('[1]Complete Route Listing'!C11=0," ",'[1]Complete Route Listing'!C11)</f>
         <v>yellow</v>
       </c>
-      <c r="C3" s="12">
-        <f>IF('[1]Complete Route Listing'!D298=0," ",'[1]Complete Route Listing'!D298)</f>
-        <v>3</v>
+      <c r="C3" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D11=0," ",'[1]Complete Route Listing'!D11)</f>
+        <v>3+</v>
       </c>
       <c r="D3" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F11=0," ",'[1]Complete Route Listing'!F11)</f>
@@ -3169,9 +3169,9 @@
         <f>IF('[1]Complete Route Listing'!C12=0," ",'[1]Complete Route Listing'!C12)</f>
         <v>#REF!</v>
       </c>
-      <c r="C4" s="12">
-        <f>IF('[1]Complete Route Listing'!D300=0," ",'[1]Complete Route Listing'!D300)</f>
-        <v>3</v>
+      <c r="C4" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D12=0," ",'[1]Complete Route Listing'!D12)</f>
+        <v>#REF!</v>
       </c>
       <c r="D4" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F12=0," ",'[1]Complete Route Listing'!F12)</f>
@@ -3189,9 +3189,9 @@
         <f>IF('[1]Complete Route Listing'!C13=0," ",'[1]Complete Route Listing'!C13)</f>
         <v>#REF!</v>
       </c>
-      <c r="C5" s="12">
-        <f>IF('[1]Complete Route Listing'!D30=0," ",'[1]Complete Route Listing'!D30)</f>
-        <v>4</v>
+      <c r="C5" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D13=0," ",'[1]Complete Route Listing'!D13)</f>
+        <v>#REF!</v>
       </c>
       <c r="D5" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F13=0," ",'[1]Complete Route Listing'!F13)</f>
@@ -3210,8 +3210,8 @@
         <v>blue</v>
       </c>
       <c r="C6" s="12">
-        <f>IF('[1]Complete Route Listing'!D38=0," ",'[1]Complete Route Listing'!D38)</f>
-        <v>4</v>
+        <f>IF('[1]Complete Route Listing'!D14=0," ",'[1]Complete Route Listing'!D14)</f>
+        <v>3</v>
       </c>
       <c r="D6" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F14=0," ",'[1]Complete Route Listing'!F14)</f>
@@ -3230,8 +3230,8 @@
         <v>orange</v>
       </c>
       <c r="C7" s="12">
-        <f>IF('[1]Complete Route Listing'!D66=0," ",'[1]Complete Route Listing'!D66)</f>
-        <v>4</v>
+        <f>IF('[1]Complete Route Listing'!D15=0," ",'[1]Complete Route Listing'!D15)</f>
+        <v>5</v>
       </c>
       <c r="D7" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F15=0," ",'[1]Complete Route Listing'!F15)</f>
@@ -3249,9 +3249,9 @@
         <f>IF('[1]Complete Route Listing'!C16=0," ",'[1]Complete Route Listing'!C16)</f>
         <v>#REF!</v>
       </c>
-      <c r="C8" s="12">
-        <f>IF('[1]Complete Route Listing'!D75=0," ",'[1]Complete Route Listing'!D75)</f>
-        <v>4</v>
+      <c r="C8" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D16=0," ",'[1]Complete Route Listing'!D16)</f>
+        <v>#REF!</v>
       </c>
       <c r="D8" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F16=0," ",'[1]Complete Route Listing'!F16)</f>
@@ -3269,9 +3269,9 @@
         <f>IF('[1]Complete Route Listing'!C17=0," ",'[1]Complete Route Listing'!C17)</f>
         <v>#REF!</v>
       </c>
-      <c r="C9" s="12">
-        <f>IF('[1]Complete Route Listing'!D104=0," ",'[1]Complete Route Listing'!D104)</f>
-        <v>4</v>
+      <c r="C9" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D17=0," ",'[1]Complete Route Listing'!D17)</f>
+        <v>#REF!</v>
       </c>
       <c r="D9" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F17=0," ",'[1]Complete Route Listing'!F17)</f>
@@ -3289,9 +3289,9 @@
         <f>IF('[1]Complete Route Listing'!C18=0," ",'[1]Complete Route Listing'!C18)</f>
         <v>green</v>
       </c>
-      <c r="C10" s="12">
-        <f>IF('[1]Complete Route Listing'!D257=0," ",'[1]Complete Route Listing'!D257)</f>
-        <v>4</v>
+      <c r="C10" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D18=0," ",'[1]Complete Route Listing'!D18)</f>
+        <v>3+</v>
       </c>
       <c r="D10" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F18=0," ",'[1]Complete Route Listing'!F18)</f>
@@ -3309,9 +3309,9 @@
         <f>IF('[1]Complete Route Listing'!C19=0," ",'[1]Complete Route Listing'!C19)</f>
         <v>red</v>
       </c>
-      <c r="C11" s="12">
-        <f>IF('[1]Complete Route Listing'!D257=0," ",'[1]Complete Route Listing'!D257)</f>
-        <v>4</v>
+      <c r="C11" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D19=0," ",'[1]Complete Route Listing'!D19)</f>
+        <v>4+</v>
       </c>
       <c r="D11" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F19=0," ",'[1]Complete Route Listing'!F19)</f>
@@ -3329,9 +3329,9 @@
         <f>IF('[1]Complete Route Listing'!C20=0," ",'[1]Complete Route Listing'!C20)</f>
         <v>#REF!</v>
       </c>
-      <c r="C12" s="12">
-        <f>IF('[1]Complete Route Listing'!D274=0," ",'[1]Complete Route Listing'!D274)</f>
-        <v>4</v>
+      <c r="C12" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D20=0," ",'[1]Complete Route Listing'!D20)</f>
+        <v>#REF!</v>
       </c>
       <c r="D12" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F20=0," ",'[1]Complete Route Listing'!F20)</f>
@@ -3349,9 +3349,9 @@
         <f>IF('[1]Complete Route Listing'!C21=0," ",'[1]Complete Route Listing'!C21)</f>
         <v>#REF!</v>
       </c>
-      <c r="C13" s="12">
-        <f>IF('[1]Complete Route Listing'!D280=0," ",'[1]Complete Route Listing'!D280)</f>
-        <v>4</v>
+      <c r="C13" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D21=0," ",'[1]Complete Route Listing'!D21)</f>
+        <v>#REF!</v>
       </c>
       <c r="D13" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F21=0," ",'[1]Complete Route Listing'!F21)</f>
@@ -3369,9 +3369,9 @@
         <f>IF('[1]Complete Route Listing'!C22=0," ",'[1]Complete Route Listing'!C22)</f>
         <v>pink</v>
       </c>
-      <c r="C14" s="12">
-        <f>IF('[1]Complete Route Listing'!D288=0," ",'[1]Complete Route Listing'!D288)</f>
-        <v>4</v>
+      <c r="C14" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D22=0," ",'[1]Complete Route Listing'!D22)</f>
+        <v>3+</v>
       </c>
       <c r="D14" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F22=0," ",'[1]Complete Route Listing'!F22)</f>
@@ -3389,9 +3389,9 @@
         <f>IF('[1]Complete Route Listing'!C23=0," ",'[1]Complete Route Listing'!C23)</f>
         <v>black</v>
       </c>
-      <c r="C15" s="12">
-        <f>IF('[1]Complete Route Listing'!D291=0," ",'[1]Complete Route Listing'!D291)</f>
-        <v>4</v>
+      <c r="C15" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D23=0," ",'[1]Complete Route Listing'!D23)</f>
+        <v>6a</v>
       </c>
       <c r="D15" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F23=0," ",'[1]Complete Route Listing'!F23)</f>
@@ -3409,9 +3409,9 @@
         <f>IF('[1]Complete Route Listing'!C24=0," ",'[1]Complete Route Listing'!C24)</f>
         <v>#REF!</v>
       </c>
-      <c r="C16" s="12">
-        <f>IF('[1]Complete Route Listing'!D299=0," ",'[1]Complete Route Listing'!D299)</f>
-        <v>4</v>
+      <c r="C16" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D24=0," ",'[1]Complete Route Listing'!D24)</f>
+        <v>#REF!</v>
       </c>
       <c r="D16" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F24=0," ",'[1]Complete Route Listing'!F24)</f>
@@ -3429,9 +3429,9 @@
         <f>IF('[1]Complete Route Listing'!C25=0," ",'[1]Complete Route Listing'!C25)</f>
         <v>#REF!</v>
       </c>
-      <c r="C17" s="12">
-        <f>IF('[1]Complete Route Listing'!D15=0," ",'[1]Complete Route Listing'!D15)</f>
-        <v>5</v>
+      <c r="C17" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D25=0," ",'[1]Complete Route Listing'!D25)</f>
+        <v>#REF!</v>
       </c>
       <c r="D17" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F25=0," ",'[1]Complete Route Listing'!F25)</f>
@@ -3449,9 +3449,9 @@
         <f>IF('[1]Complete Route Listing'!C26=0," ",'[1]Complete Route Listing'!C26)</f>
         <v>orange</v>
       </c>
-      <c r="C18" s="12">
-        <f>IF('[1]Complete Route Listing'!D34=0," ",'[1]Complete Route Listing'!D34)</f>
-        <v>5</v>
+      <c r="C18" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D26=0," ",'[1]Complete Route Listing'!D26)</f>
+        <v>3+</v>
       </c>
       <c r="D18" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F26=0," ",'[1]Complete Route Listing'!F26)</f>
@@ -3469,9 +3469,9 @@
         <f>IF('[1]Complete Route Listing'!C27=0," ",'[1]Complete Route Listing'!C27)</f>
         <v>flo yellow</v>
       </c>
-      <c r="C19" s="12">
-        <f>IF('[1]Complete Route Listing'!D39=0," ",'[1]Complete Route Listing'!D39)</f>
-        <v>5</v>
+      <c r="C19" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D27=0," ",'[1]Complete Route Listing'!D27)</f>
+        <v>6a</v>
       </c>
       <c r="D19" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F27=0," ",'[1]Complete Route Listing'!F27)</f>
@@ -3489,9 +3489,9 @@
         <f>IF('[1]Complete Route Listing'!C28=0," ",'[1]Complete Route Listing'!C28)</f>
         <v>#REF!</v>
       </c>
-      <c r="C20" s="12">
-        <f>IF('[1]Complete Route Listing'!D43=0," ",'[1]Complete Route Listing'!D43)</f>
-        <v>5</v>
+      <c r="C20" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D28=0," ",'[1]Complete Route Listing'!D28)</f>
+        <v>#REF!</v>
       </c>
       <c r="D20" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F28=0," ",'[1]Complete Route Listing'!F28)</f>
@@ -3509,9 +3509,9 @@
         <f>IF('[1]Complete Route Listing'!C29=0," ",'[1]Complete Route Listing'!C29)</f>
         <v>#REF!</v>
       </c>
-      <c r="C21" s="12">
-        <f>IF('[1]Complete Route Listing'!D46=0," ",'[1]Complete Route Listing'!D46)</f>
-        <v>5</v>
+      <c r="C21" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D29=0," ",'[1]Complete Route Listing'!D29)</f>
+        <v>#REF!</v>
       </c>
       <c r="D21" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F29=0," ",'[1]Complete Route Listing'!F29)</f>
@@ -3530,8 +3530,8 @@
         <v>green</v>
       </c>
       <c r="C22" s="12">
-        <f>IF('[1]Complete Route Listing'!D50=0," ",'[1]Complete Route Listing'!D50)</f>
-        <v>5</v>
+        <f>IF('[1]Complete Route Listing'!D30=0," ",'[1]Complete Route Listing'!D30)</f>
+        <v>4</v>
       </c>
       <c r="D22" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F30=0," ",'[1]Complete Route Listing'!F30)</f>
@@ -3549,9 +3549,9 @@
         <f>IF('[1]Complete Route Listing'!C31=0," ",'[1]Complete Route Listing'!C31)</f>
         <v>blue</v>
       </c>
-      <c r="C23" s="12">
-        <f>IF('[1]Complete Route Listing'!D111=0," ",'[1]Complete Route Listing'!D111)</f>
-        <v>5</v>
+      <c r="C23" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D31=0," ",'[1]Complete Route Listing'!D31)</f>
+        <v>6a</v>
       </c>
       <c r="D23" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F31=0," ",'[1]Complete Route Listing'!F31)</f>
@@ -3569,9 +3569,9 @@
         <f>IF('[1]Complete Route Listing'!C32=0," ",'[1]Complete Route Listing'!C32)</f>
         <v>#REF!</v>
       </c>
-      <c r="C24" s="12">
-        <f>IF('[1]Complete Route Listing'!D138=0," ",'[1]Complete Route Listing'!D138)</f>
-        <v>5</v>
+      <c r="C24" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D32=0," ",'[1]Complete Route Listing'!D32)</f>
+        <v>#REF!</v>
       </c>
       <c r="D24" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F32=0," ",'[1]Complete Route Listing'!F32)</f>
@@ -3589,9 +3589,9 @@
         <f>IF('[1]Complete Route Listing'!C33=0," ",'[1]Complete Route Listing'!C33)</f>
         <v>#REF!</v>
       </c>
-      <c r="C25" s="12">
-        <f>IF('[1]Complete Route Listing'!D152=0," ",'[1]Complete Route Listing'!D152)</f>
-        <v>5</v>
+      <c r="C25" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D33=0," ",'[1]Complete Route Listing'!D33)</f>
+        <v>#REF!</v>
       </c>
       <c r="D25" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F33=0," ",'[1]Complete Route Listing'!F33)</f>
@@ -3610,7 +3610,7 @@
         <v xml:space="preserve">black </v>
       </c>
       <c r="C26" s="12">
-        <f>IF('[1]Complete Route Listing'!D248=0," ",'[1]Complete Route Listing'!D248)</f>
+        <f>IF('[1]Complete Route Listing'!D34=0," ",'[1]Complete Route Listing'!D34)</f>
         <v>5</v>
       </c>
       <c r="D26" s="13" t="str">
@@ -3629,9 +3629,9 @@
         <f>IF('[1]Complete Route Listing'!C35=0," ",'[1]Complete Route Listing'!C35)</f>
         <v>pink</v>
       </c>
-      <c r="C27" s="12">
-        <f>IF('[1]Complete Route Listing'!D62=0," ",'[1]Complete Route Listing'!D62)</f>
-        <v>5</v>
+      <c r="C27" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D35=0," ",'[1]Complete Route Listing'!D35)</f>
+        <v>6a</v>
       </c>
       <c r="D27" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F35=0," ",'[1]Complete Route Listing'!F35)</f>
@@ -3649,9 +3649,9 @@
         <f>IF('[1]Complete Route Listing'!C36=0," ",'[1]Complete Route Listing'!C36)</f>
         <v>#REF!</v>
       </c>
-      <c r="C28" s="12">
-        <f>IF('[1]Complete Route Listing'!D70=0," ",'[1]Complete Route Listing'!D70)</f>
-        <v>5</v>
+      <c r="C28" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D36=0," ",'[1]Complete Route Listing'!D36)</f>
+        <v>#REF!</v>
       </c>
       <c r="D28" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F36=0," ",'[1]Complete Route Listing'!F36)</f>
@@ -3669,9 +3669,9 @@
         <f>IF('[1]Complete Route Listing'!C37=0," ",'[1]Complete Route Listing'!C37)</f>
         <v>#REF!</v>
       </c>
-      <c r="C29" s="12">
-        <f>IF('[1]Complete Route Listing'!D74=0," ",'[1]Complete Route Listing'!D74)</f>
-        <v>5</v>
+      <c r="C29" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D37=0," ",'[1]Complete Route Listing'!D37)</f>
+        <v>#REF!</v>
       </c>
       <c r="D29" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F37=0," ",'[1]Complete Route Listing'!F37)</f>
@@ -3690,8 +3690,8 @@
         <v>flo yellow</v>
       </c>
       <c r="C30" s="12">
-        <f>IF('[1]Complete Route Listing'!D80=0," ",'[1]Complete Route Listing'!D80)</f>
-        <v>5</v>
+        <f>IF('[1]Complete Route Listing'!D38=0," ",'[1]Complete Route Listing'!D38)</f>
+        <v>4</v>
       </c>
       <c r="D30" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F38=0," ",'[1]Complete Route Listing'!F38)</f>
@@ -3710,7 +3710,7 @@
         <v>green</v>
       </c>
       <c r="C31" s="12">
-        <f>IF('[1]Complete Route Listing'!D83=0," ",'[1]Complete Route Listing'!D83)</f>
+        <f>IF('[1]Complete Route Listing'!D39=0," ",'[1]Complete Route Listing'!D39)</f>
         <v>5</v>
       </c>
       <c r="D31" s="13" t="str">
@@ -3729,9 +3729,9 @@
         <f>IF('[1]Complete Route Listing'!C40=0," ",'[1]Complete Route Listing'!C40)</f>
         <v>#REF!</v>
       </c>
-      <c r="C32" s="12">
-        <f>IF('[1]Complete Route Listing'!D177=0," ",'[1]Complete Route Listing'!D177)</f>
-        <v>5</v>
+      <c r="C32" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D40=0," ",'[1]Complete Route Listing'!D40)</f>
+        <v>#REF!</v>
       </c>
       <c r="D32" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F40=0," ",'[1]Complete Route Listing'!F40)</f>
@@ -3749,9 +3749,9 @@
         <f>IF('[1]Complete Route Listing'!C41=0," ",'[1]Complete Route Listing'!C41)</f>
         <v>#REF!</v>
       </c>
-      <c r="C33" s="12">
-        <f>IF('[1]Complete Route Listing'!D177=0," ",'[1]Complete Route Listing'!D177)</f>
-        <v>5</v>
+      <c r="C33" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D41=0," ",'[1]Complete Route Listing'!D41)</f>
+        <v>#REF!</v>
       </c>
       <c r="D33" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F41=0," ",'[1]Complete Route Listing'!F41)</f>
@@ -3769,9 +3769,9 @@
         <f>IF('[1]Complete Route Listing'!C42=0," ",'[1]Complete Route Listing'!C42)</f>
         <v>red</v>
       </c>
-      <c r="C34" s="12">
-        <f>IF('[1]Complete Route Listing'!D259=0," ",'[1]Complete Route Listing'!D259)</f>
-        <v>5</v>
+      <c r="C34" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D42=0," ",'[1]Complete Route Listing'!D42)</f>
+        <v>4+</v>
       </c>
       <c r="D34" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F42=0," ",'[1]Complete Route Listing'!F42)</f>
@@ -3790,7 +3790,7 @@
         <v>blue</v>
       </c>
       <c r="C35" s="12">
-        <f>IF('[1]Complete Route Listing'!D286=0," ",'[1]Complete Route Listing'!D286)</f>
+        <f>IF('[1]Complete Route Listing'!D43=0," ",'[1]Complete Route Listing'!D43)</f>
         <v>5</v>
       </c>
       <c r="D35" s="13" t="str">
@@ -3809,9 +3809,9 @@
         <f>IF('[1]Complete Route Listing'!C44=0," ",'[1]Complete Route Listing'!C44)</f>
         <v>#REF!</v>
       </c>
-      <c r="C36" s="12">
-        <f>IF('[1]Complete Route Listing'!D295=0," ",'[1]Complete Route Listing'!D295)</f>
-        <v>5</v>
+      <c r="C36" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D44=0," ",'[1]Complete Route Listing'!D44)</f>
+        <v>#REF!</v>
       </c>
       <c r="D36" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F44=0," ",'[1]Complete Route Listing'!F44)</f>
@@ -3829,9 +3829,9 @@
         <f>IF('[1]Complete Route Listing'!C45=0," ",'[1]Complete Route Listing'!C45)</f>
         <v>#REF!</v>
       </c>
-      <c r="C37" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D10=0," ",'[1]Complete Route Listing'!D10)</f>
-        <v>3+</v>
+      <c r="C37" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D45=0," ",'[1]Complete Route Listing'!D45)</f>
+        <v>#REF!</v>
       </c>
       <c r="D37" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F45=0," ",'[1]Complete Route Listing'!F45)</f>
@@ -3849,9 +3849,9 @@
         <f>IF('[1]Complete Route Listing'!C46=0," ",'[1]Complete Route Listing'!C46)</f>
         <v>pink</v>
       </c>
-      <c r="C38" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D11=0," ",'[1]Complete Route Listing'!D11)</f>
-        <v>3+</v>
+      <c r="C38" s="12">
+        <f>IF('[1]Complete Route Listing'!D46=0," ",'[1]Complete Route Listing'!D46)</f>
+        <v>5</v>
       </c>
       <c r="D38" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F46=0," ",'[1]Complete Route Listing'!F46)</f>
@@ -3870,8 +3870,8 @@
         <v>black</v>
       </c>
       <c r="C39" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D18=0," ",'[1]Complete Route Listing'!D18)</f>
-        <v>3+</v>
+        <f>IF('[1]Complete Route Listing'!D47=0," ",'[1]Complete Route Listing'!D47)</f>
+        <v>5+</v>
       </c>
       <c r="D39" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F47=0," ",'[1]Complete Route Listing'!F47)</f>
@@ -3889,9 +3889,9 @@
         <f>IF('[1]Complete Route Listing'!C48=0," ",'[1]Complete Route Listing'!C48)</f>
         <v>#REF!</v>
       </c>
-      <c r="C40" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D22=0," ",'[1]Complete Route Listing'!D22)</f>
-        <v>3+</v>
+      <c r="C40" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D48=0," ",'[1]Complete Route Listing'!D48)</f>
+        <v>#REF!</v>
       </c>
       <c r="D40" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F48=0," ",'[1]Complete Route Listing'!F48)</f>
@@ -3909,9 +3909,9 @@
         <f>IF('[1]Complete Route Listing'!C49=0," ",'[1]Complete Route Listing'!C49)</f>
         <v>#REF!</v>
       </c>
-      <c r="C41" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D26=0," ",'[1]Complete Route Listing'!D26)</f>
-        <v>3+</v>
+      <c r="C41" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D49=0," ",'[1]Complete Route Listing'!D49)</f>
+        <v>#REF!</v>
       </c>
       <c r="D41" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F49=0," ",'[1]Complete Route Listing'!F49)</f>
@@ -3929,9 +3929,9 @@
         <f>IF('[1]Complete Route Listing'!C50=0," ",'[1]Complete Route Listing'!C50)</f>
         <v>orange</v>
       </c>
-      <c r="C42" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D19=0," ",'[1]Complete Route Listing'!D19)</f>
-        <v>4+</v>
+      <c r="C42" s="12">
+        <f>IF('[1]Complete Route Listing'!D50=0," ",'[1]Complete Route Listing'!D50)</f>
+        <v>5</v>
       </c>
       <c r="D42" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F50=0," ",'[1]Complete Route Listing'!F50)</f>
@@ -3950,8 +3950,8 @@
         <v>yellow</v>
       </c>
       <c r="C43" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D42=0," ",'[1]Complete Route Listing'!D42)</f>
-        <v>4+</v>
+        <f>IF('[1]Complete Route Listing'!D51=0," ",'[1]Complete Route Listing'!D51)</f>
+        <v>6b+</v>
       </c>
       <c r="D43" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F51=0," ",'[1]Complete Route Listing'!F51)</f>
@@ -3969,9 +3969,9 @@
         <f>IF('[1]Complete Route Listing'!C52=0," ",'[1]Complete Route Listing'!C52)</f>
         <v>#REF!</v>
       </c>
-      <c r="C44" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D120=0," ",'[1]Complete Route Listing'!D120)</f>
-        <v>4+</v>
+      <c r="C44" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D52=0," ",'[1]Complete Route Listing'!D52)</f>
+        <v>#REF!</v>
       </c>
       <c r="D44" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F52=0," ",'[1]Complete Route Listing'!F52)</f>
@@ -3989,9 +3989,9 @@
         <f>IF('[1]Complete Route Listing'!C53=0," ",'[1]Complete Route Listing'!C53)</f>
         <v>#REF!</v>
       </c>
-      <c r="C45" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D241=0," ",'[1]Complete Route Listing'!D241)</f>
-        <v>4+</v>
+      <c r="C45" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D53=0," ",'[1]Complete Route Listing'!D53)</f>
+        <v>#REF!</v>
       </c>
       <c r="D45" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F53=0," ",'[1]Complete Route Listing'!F53)</f>
@@ -4010,8 +4010,8 @@
         <v>green</v>
       </c>
       <c r="C46" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D250=0," ",'[1]Complete Route Listing'!D250)</f>
-        <v>4+</v>
+        <f>IF('[1]Complete Route Listing'!D54=0," ",'[1]Complete Route Listing'!D54)</f>
+        <v>5+</v>
       </c>
       <c r="D46" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F54=0," ",'[1]Complete Route Listing'!F54)</f>
@@ -4030,8 +4030,8 @@
         <v>black</v>
       </c>
       <c r="C47" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D92=0," ",'[1]Complete Route Listing'!D92)</f>
-        <v>4+</v>
+        <f>IF('[1]Complete Route Listing'!D55=0," ",'[1]Complete Route Listing'!D55)</f>
+        <v>6a</v>
       </c>
       <c r="D47" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F55=0," ",'[1]Complete Route Listing'!F55)</f>
@@ -4049,9 +4049,9 @@
         <f>IF('[1]Complete Route Listing'!C56=0," ",'[1]Complete Route Listing'!C56)</f>
         <v>#REF!</v>
       </c>
-      <c r="C48" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D268=0," ",'[1]Complete Route Listing'!D268)</f>
-        <v>4+</v>
+      <c r="C48" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D56=0," ",'[1]Complete Route Listing'!D56)</f>
+        <v>#REF!</v>
       </c>
       <c r="D48" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F56=0," ",'[1]Complete Route Listing'!F56)</f>
@@ -4069,9 +4069,9 @@
         <f>IF('[1]Complete Route Listing'!C57=0," ",'[1]Complete Route Listing'!C57)</f>
         <v>#REF!</v>
       </c>
-      <c r="C49" s="17" t="str">
-        <f>IF('[1]Complete Route Listing'!D272=0," ",'[1]Complete Route Listing'!D272)</f>
-        <v>4+</v>
+      <c r="C49" s="17" t="e">
+        <f>IF('[1]Complete Route Listing'!D57=0," ",'[1]Complete Route Listing'!D57)</f>
+        <v>#REF!</v>
       </c>
       <c r="D49" s="18" t="e">
         <f>IF('[1]Complete Route Listing'!F57=0," ",'[1]Complete Route Listing'!F57)</f>
@@ -4090,8 +4090,8 @@
         <v>white</v>
       </c>
       <c r="C50" s="7" t="str">
-        <f>IF('[1]Complete Route Listing'!D282=0," ",'[1]Complete Route Listing'!D282)</f>
-        <v>4+</v>
+        <f>IF('[1]Complete Route Listing'!D106=0," ",'[1]Complete Route Listing'!D106)</f>
+        <v>6c</v>
       </c>
       <c r="D50" s="8" t="str">
         <f>IF('[1]Complete Route Listing'!F106=0," ",'[1]Complete Route Listing'!F106)</f>
@@ -4110,8 +4110,8 @@
         <v>purple</v>
       </c>
       <c r="C51" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D47=0," ",'[1]Complete Route Listing'!D47)</f>
-        <v>5+</v>
+        <f>IF('[1]Complete Route Listing'!D107=0," ",'[1]Complete Route Listing'!D107)</f>
+        <v>6b</v>
       </c>
       <c r="D51" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F107=0," ",'[1]Complete Route Listing'!F107)</f>
@@ -4130,8 +4130,8 @@
         <v>orange</v>
       </c>
       <c r="C52" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D54=0," ",'[1]Complete Route Listing'!D54)</f>
-        <v>5+</v>
+        <f>IF('[1]Complete Route Listing'!D108=0," ",'[1]Complete Route Listing'!D108)</f>
+        <v>6c</v>
       </c>
       <c r="D52" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F108=0," ",'[1]Complete Route Listing'!F108)</f>
@@ -4149,9 +4149,9 @@
         <f>IF('[1]Complete Route Listing'!C109=0," ",'[1]Complete Route Listing'!C109)</f>
         <v>#REF!</v>
       </c>
-      <c r="C53" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D115=0," ",'[1]Complete Route Listing'!D115)</f>
-        <v>5+</v>
+      <c r="C53" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D109=0," ",'[1]Complete Route Listing'!D109)</f>
+        <v>#REF!</v>
       </c>
       <c r="D53" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F109=0," ",'[1]Complete Route Listing'!F109)</f>
@@ -4170,8 +4170,8 @@
         <v>yellow</v>
       </c>
       <c r="C54" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D240=0," ",'[1]Complete Route Listing'!D240)</f>
-        <v>5+</v>
+        <f>IF('[1]Complete Route Listing'!D110=0," ",'[1]Complete Route Listing'!D110)</f>
+        <v>6b+</v>
       </c>
       <c r="D54" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F110=0," ",'[1]Complete Route Listing'!F110)</f>
@@ -4189,9 +4189,9 @@
         <f>IF('[1]Complete Route Listing'!C111=0," ",'[1]Complete Route Listing'!C111)</f>
         <v>red</v>
       </c>
-      <c r="C55" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D76=0," ",'[1]Complete Route Listing'!D76)</f>
-        <v>5+</v>
+      <c r="C55" s="12">
+        <f>IF('[1]Complete Route Listing'!D111=0," ",'[1]Complete Route Listing'!D111)</f>
+        <v>5</v>
       </c>
       <c r="D55" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F111=0," ",'[1]Complete Route Listing'!F111)</f>
@@ -4209,9 +4209,9 @@
         <f>IF('[1]Complete Route Listing'!C112=0," ",'[1]Complete Route Listing'!C112)</f>
         <v>#REF!</v>
       </c>
-      <c r="C56" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D85=0," ",'[1]Complete Route Listing'!D85)</f>
-        <v>5+</v>
+      <c r="C56" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D112=0," ",'[1]Complete Route Listing'!D112)</f>
+        <v>#REF!</v>
       </c>
       <c r="D56" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F112=0," ",'[1]Complete Route Listing'!F112)</f>
@@ -4229,9 +4229,9 @@
         <f>IF('[1]Complete Route Listing'!C113=0," ",'[1]Complete Route Listing'!C113)</f>
         <v>#REF!</v>
       </c>
-      <c r="C57" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D88=0," ",'[1]Complete Route Listing'!D88)</f>
-        <v>5+</v>
+      <c r="C57" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D113=0," ",'[1]Complete Route Listing'!D113)</f>
+        <v>#REF!</v>
       </c>
       <c r="D57" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F113=0," ",'[1]Complete Route Listing'!F113)</f>
@@ -4250,8 +4250,8 @@
         <v>blue</v>
       </c>
       <c r="C58" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D91=0," ",'[1]Complete Route Listing'!D91)</f>
-        <v>5+</v>
+        <f>IF('[1]Complete Route Listing'!D114=0," ",'[1]Complete Route Listing'!D114)</f>
+        <v>6b</v>
       </c>
       <c r="D58" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F114=0," ",'[1]Complete Route Listing'!F114)</f>
@@ -4270,7 +4270,7 @@
         <v>green</v>
       </c>
       <c r="C59" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D102=0," ",'[1]Complete Route Listing'!D102)</f>
+        <f>IF('[1]Complete Route Listing'!D115=0," ",'[1]Complete Route Listing'!D115)</f>
         <v>5+</v>
       </c>
       <c r="D59" s="13" t="str">
@@ -4289,9 +4289,9 @@
         <f>IF('[1]Complete Route Listing'!C116=0," ",'[1]Complete Route Listing'!C116)</f>
         <v>#REF!</v>
       </c>
-      <c r="C60" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D178=0," ",'[1]Complete Route Listing'!D178)</f>
-        <v>5+</v>
+      <c r="C60" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D116=0," ",'[1]Complete Route Listing'!D116)</f>
+        <v>#REF!</v>
       </c>
       <c r="D60" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F116=0," ",'[1]Complete Route Listing'!F116)</f>
@@ -4309,9 +4309,9 @@
         <f>IF('[1]Complete Route Listing'!C117=0," ",'[1]Complete Route Listing'!C117)</f>
         <v>#REF!</v>
       </c>
-      <c r="C61" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D183=0," ",'[1]Complete Route Listing'!D183)</f>
-        <v>5+</v>
+      <c r="C61" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D117=0," ",'[1]Complete Route Listing'!D117)</f>
+        <v>#REF!</v>
       </c>
       <c r="D61" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F117=0," ",'[1]Complete Route Listing'!F117)</f>
@@ -4330,8 +4330,8 @@
         <v>flo yellow</v>
       </c>
       <c r="C62" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D264=0," ",'[1]Complete Route Listing'!D264)</f>
-        <v>5+</v>
+        <f>IF('[1]Complete Route Listing'!D118=0," ",'[1]Complete Route Listing'!D118)</f>
+        <v>6a</v>
       </c>
       <c r="D62" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F118=0," ",'[1]Complete Route Listing'!F118)</f>
@@ -4350,8 +4350,8 @@
         <v>purple</v>
       </c>
       <c r="C63" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D290=0," ",'[1]Complete Route Listing'!D290)</f>
-        <v>5+</v>
+        <f>IF('[1]Complete Route Listing'!D119=0," ",'[1]Complete Route Listing'!D119)</f>
+        <v>6b+</v>
       </c>
       <c r="D63" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F119=0," ",'[1]Complete Route Listing'!F119)</f>
@@ -4370,8 +4370,8 @@
         <v>white</v>
       </c>
       <c r="C64" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D23=0," ",'[1]Complete Route Listing'!D23)</f>
-        <v>6a</v>
+        <f>IF('[1]Complete Route Listing'!D120=0," ",'[1]Complete Route Listing'!D120)</f>
+        <v>4+</v>
       </c>
       <c r="D64" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F120=0," ",'[1]Complete Route Listing'!F120)</f>
@@ -4389,9 +4389,9 @@
         <f>IF('[1]Complete Route Listing'!C121=0," ",'[1]Complete Route Listing'!C121)</f>
         <v>#REF!</v>
       </c>
-      <c r="C65" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D27=0," ",'[1]Complete Route Listing'!D27)</f>
-        <v>6a</v>
+      <c r="C65" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D121=0," ",'[1]Complete Route Listing'!D121)</f>
+        <v>#REF!</v>
       </c>
       <c r="D65" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F121=0," ",'[1]Complete Route Listing'!F121)</f>
@@ -4410,8 +4410,8 @@
         <v>orange</v>
       </c>
       <c r="C66" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D31=0," ",'[1]Complete Route Listing'!D31)</f>
-        <v>6a</v>
+        <f>IF('[1]Complete Route Listing'!D122=0," ",'[1]Complete Route Listing'!D122)</f>
+        <v>7a+</v>
       </c>
       <c r="D66" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F122=0," ",'[1]Complete Route Listing'!F122)</f>
@@ -4430,7 +4430,7 @@
         <v>pink</v>
       </c>
       <c r="C67" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D35=0," ",'[1]Complete Route Listing'!D35)</f>
+        <f>IF('[1]Complete Route Listing'!D123=0," ",'[1]Complete Route Listing'!D123)</f>
         <v>6a</v>
       </c>
       <c r="D67" s="13" t="str">
@@ -4449,9 +4449,9 @@
         <f>IF('[1]Complete Route Listing'!C124=0," ",'[1]Complete Route Listing'!C124)</f>
         <v>#REF!</v>
       </c>
-      <c r="C68" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D55=0," ",'[1]Complete Route Listing'!D55)</f>
-        <v>6a</v>
+      <c r="C68" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D124=0," ",'[1]Complete Route Listing'!D124)</f>
+        <v>#REF!</v>
       </c>
       <c r="D68" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F124=0," ",'[1]Complete Route Listing'!F124)</f>
@@ -4469,9 +4469,9 @@
         <f>IF('[1]Complete Route Listing'!C125=0," ",'[1]Complete Route Listing'!C125)</f>
         <v>#REF!</v>
       </c>
-      <c r="C69" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D118=0," ",'[1]Complete Route Listing'!D118)</f>
-        <v>6a</v>
+      <c r="C69" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D125=0," ",'[1]Complete Route Listing'!D125)</f>
+        <v>#REF!</v>
       </c>
       <c r="D69" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F125=0," ",'[1]Complete Route Listing'!F125)</f>
@@ -4490,8 +4490,8 @@
         <v>red</v>
       </c>
       <c r="C70" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D123=0," ",'[1]Complete Route Listing'!D123)</f>
-        <v>6a</v>
+        <f>IF('[1]Complete Route Listing'!D126=0," ",'[1]Complete Route Listing'!D126)</f>
+        <v>7b</v>
       </c>
       <c r="D70" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F126=0," ",'[1]Complete Route Listing'!F126)</f>
@@ -4510,8 +4510,8 @@
         <v>black</v>
       </c>
       <c r="C71" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D131=0," ",'[1]Complete Route Listing'!D131)</f>
-        <v>6a</v>
+        <f>IF('[1]Complete Route Listing'!D127=0," ",'[1]Complete Route Listing'!D127)</f>
+        <v>7b</v>
       </c>
       <c r="D71" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F127=0," ",'[1]Complete Route Listing'!F127)</f>
@@ -4530,8 +4530,8 @@
         <v>purple</v>
       </c>
       <c r="C72" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D134=0," ",'[1]Complete Route Listing'!D134)</f>
-        <v>6a</v>
+        <f>IF('[1]Complete Route Listing'!D128=0," ",'[1]Complete Route Listing'!D128)</f>
+        <v>7a</v>
       </c>
       <c r="D72" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F128=0," ",'[1]Complete Route Listing'!F128)</f>
@@ -4549,9 +4549,9 @@
         <f>IF('[1]Complete Route Listing'!C129=0," ",'[1]Complete Route Listing'!C129)</f>
         <v>#REF!</v>
       </c>
-      <c r="C73" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D135=0," ",'[1]Complete Route Listing'!D135)</f>
-        <v>6a</v>
+      <c r="C73" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D129=0," ",'[1]Complete Route Listing'!D129)</f>
+        <v>#REF!</v>
       </c>
       <c r="D73" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F129=0," ",'[1]Complete Route Listing'!F129)</f>
@@ -4570,8 +4570,8 @@
         <v>green</v>
       </c>
       <c r="C74" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D151=0," ",'[1]Complete Route Listing'!D151)</f>
-        <v>6a</v>
+        <f>IF('[1]Complete Route Listing'!D130=0," ",'[1]Complete Route Listing'!D130)</f>
+        <v>7b+</v>
       </c>
       <c r="D74" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F130=0," ",'[1]Complete Route Listing'!F130)</f>
@@ -4590,7 +4590,7 @@
         <v>orange</v>
       </c>
       <c r="C75" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D242=0," ",'[1]Complete Route Listing'!D242)</f>
+        <f>IF('[1]Complete Route Listing'!D131=0," ",'[1]Complete Route Listing'!D131)</f>
         <v>6a</v>
       </c>
       <c r="D75" s="13" t="str">
@@ -4610,8 +4610,8 @@
         <v>yellow</v>
       </c>
       <c r="C76" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D58=0," ",'[1]Complete Route Listing'!D58)</f>
-        <v>6a</v>
+        <f>IF('[1]Complete Route Listing'!D132=0," ",'[1]Complete Route Listing'!D132)</f>
+        <v>6c</v>
       </c>
       <c r="D76" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F132=0," ",'[1]Complete Route Listing'!F132)</f>
@@ -4629,9 +4629,9 @@
         <f>IF('[1]Complete Route Listing'!C133=0," ",'[1]Complete Route Listing'!C133)</f>
         <v>#REF!</v>
       </c>
-      <c r="C77" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D67=0," ",'[1]Complete Route Listing'!D67)</f>
-        <v>6a</v>
+      <c r="C77" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D133=0," ",'[1]Complete Route Listing'!D133)</f>
+        <v>#REF!</v>
       </c>
       <c r="D77" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F133=0," ",'[1]Complete Route Listing'!F133)</f>
@@ -4650,7 +4650,7 @@
         <v>blue</v>
       </c>
       <c r="C78" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D84=0," ",'[1]Complete Route Listing'!D84)</f>
+        <f>IF('[1]Complete Route Listing'!D134=0," ",'[1]Complete Route Listing'!D134)</f>
         <v>6a</v>
       </c>
       <c r="D78" s="13" t="str">
@@ -4670,7 +4670,7 @@
         <v>purple</v>
       </c>
       <c r="C79" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D86=0," ",'[1]Complete Route Listing'!D86)</f>
+        <f>IF('[1]Complete Route Listing'!D135=0," ",'[1]Complete Route Listing'!D135)</f>
         <v>6a</v>
       </c>
       <c r="D79" s="13" t="str">
@@ -4689,9 +4689,9 @@
         <f>IF('[1]Complete Route Listing'!C136=0," ",'[1]Complete Route Listing'!C136)</f>
         <v>#REF!</v>
       </c>
-      <c r="C80" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D95=0," ",'[1]Complete Route Listing'!D95)</f>
-        <v>6a</v>
+      <c r="C80" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D136=0," ",'[1]Complete Route Listing'!D136)</f>
+        <v>#REF!</v>
       </c>
       <c r="D80" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F136=0," ",'[1]Complete Route Listing'!F136)</f>
@@ -4709,9 +4709,9 @@
         <f>IF('[1]Complete Route Listing'!C137=0," ",'[1]Complete Route Listing'!C137)</f>
         <v>#REF!</v>
       </c>
-      <c r="C81" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D172=0," ",'[1]Complete Route Listing'!D172)</f>
-        <v>6a</v>
+      <c r="C81" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D137=0," ",'[1]Complete Route Listing'!D137)</f>
+        <v>#REF!</v>
       </c>
       <c r="D81" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F137=0," ",'[1]Complete Route Listing'!F137)</f>
@@ -4729,9 +4729,9 @@
         <f>IF('[1]Complete Route Listing'!C138=0," ",'[1]Complete Route Listing'!C138)</f>
         <v>red</v>
       </c>
-      <c r="C82" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D186=0," ",'[1]Complete Route Listing'!D186)</f>
-        <v>6a</v>
+      <c r="C82" s="12">
+        <f>IF('[1]Complete Route Listing'!D138=0," ",'[1]Complete Route Listing'!D138)</f>
+        <v>5</v>
       </c>
       <c r="D82" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F138=0," ",'[1]Complete Route Listing'!F138)</f>
@@ -4750,8 +4750,8 @@
         <v>pink</v>
       </c>
       <c r="C83" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D192=0," ",'[1]Complete Route Listing'!D192)</f>
-        <v>6a</v>
+        <f>IF('[1]Complete Route Listing'!D139=0," ",'[1]Complete Route Listing'!D139)</f>
+        <v>6c+</v>
       </c>
       <c r="D83" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F139=0," ",'[1]Complete Route Listing'!F139)</f>
@@ -4769,9 +4769,9 @@
         <f>IF('[1]Complete Route Listing'!C140=0," ",'[1]Complete Route Listing'!C140)</f>
         <v>#REF!</v>
       </c>
-      <c r="C84" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D195=0," ",'[1]Complete Route Listing'!D195)</f>
-        <v>6a</v>
+      <c r="C84" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D140=0," ",'[1]Complete Route Listing'!D140)</f>
+        <v>#REF!</v>
       </c>
       <c r="D84" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F140=0," ",'[1]Complete Route Listing'!F140)</f>
@@ -4789,9 +4789,9 @@
         <f>IF('[1]Complete Route Listing'!C141=0," ",'[1]Complete Route Listing'!C141)</f>
         <v>#REF!</v>
       </c>
-      <c r="C85" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D198=0," ",'[1]Complete Route Listing'!D198)</f>
-        <v>6a</v>
+      <c r="C85" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D141=0," ",'[1]Complete Route Listing'!D141)</f>
+        <v>#REF!</v>
       </c>
       <c r="D85" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F141=0," ",'[1]Complete Route Listing'!F141)</f>
@@ -4810,8 +4810,8 @@
         <v>blue</v>
       </c>
       <c r="C86" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D275=0," ",'[1]Complete Route Listing'!D275)</f>
-        <v>6a</v>
+        <f>IF('[1]Complete Route Listing'!D142=0," ",'[1]Complete Route Listing'!D142)</f>
+        <v>6a+</v>
       </c>
       <c r="D86" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F142=0," ",'[1]Complete Route Listing'!F142)</f>
@@ -4830,8 +4830,8 @@
         <v>purple</v>
       </c>
       <c r="C87" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D276=0," ",'[1]Complete Route Listing'!D276)</f>
-        <v>6a</v>
+        <f>IF('[1]Complete Route Listing'!D143=0," ",'[1]Complete Route Listing'!D143)</f>
+        <v>7b+</v>
       </c>
       <c r="D87" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F143=0," ",'[1]Complete Route Listing'!F143)</f>
@@ -4850,8 +4850,8 @@
         <v>orange</v>
       </c>
       <c r="C88" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D278=0," ",'[1]Complete Route Listing'!D278)</f>
-        <v>6a</v>
+        <f>IF('[1]Complete Route Listing'!D144=0," ",'[1]Complete Route Listing'!D144)</f>
+        <v>6b</v>
       </c>
       <c r="D88" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F144=0," ",'[1]Complete Route Listing'!F144)</f>
@@ -4869,9 +4869,9 @@
         <f>IF('[1]Complete Route Listing'!C145=0," ",'[1]Complete Route Listing'!C145)</f>
         <v>#REF!</v>
       </c>
-      <c r="C89" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D283=0," ",'[1]Complete Route Listing'!D283)</f>
-        <v>6a</v>
+      <c r="C89" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D145=0," ",'[1]Complete Route Listing'!D145)</f>
+        <v>#REF!</v>
       </c>
       <c r="D89" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F145=0," ",'[1]Complete Route Listing'!F145)</f>
@@ -4890,8 +4890,8 @@
         <v>green</v>
       </c>
       <c r="C90" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D142=0," ",'[1]Complete Route Listing'!D142)</f>
-        <v>6a+</v>
+        <f>IF('[1]Complete Route Listing'!D146=0," ",'[1]Complete Route Listing'!D146)</f>
+        <v>7c</v>
       </c>
       <c r="D90" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F146=0," ",'[1]Complete Route Listing'!F146)</f>
@@ -4910,8 +4910,8 @@
         <v>flo yellow</v>
       </c>
       <c r="C91" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D148=0," ",'[1]Complete Route Listing'!D148)</f>
-        <v>6a+</v>
+        <f>IF('[1]Complete Route Listing'!D147=0," ",'[1]Complete Route Listing'!D147)</f>
+        <v>7a</v>
       </c>
       <c r="D91" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F147=0," ",'[1]Complete Route Listing'!F147)</f>
@@ -4930,7 +4930,7 @@
         <v>white</v>
       </c>
       <c r="C92" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D210=0," ",'[1]Complete Route Listing'!D210)</f>
+        <f>IF('[1]Complete Route Listing'!D148=0," ",'[1]Complete Route Listing'!D148)</f>
         <v>6a+</v>
       </c>
       <c r="D92" s="13" t="str">
@@ -4949,9 +4949,9 @@
         <f>IF('[1]Complete Route Listing'!C149=0," ",'[1]Complete Route Listing'!C149)</f>
         <v>#REF!</v>
       </c>
-      <c r="C93" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D230=0," ",'[1]Complete Route Listing'!D230)</f>
-        <v>6a+</v>
+      <c r="C93" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D149=0," ",'[1]Complete Route Listing'!D149)</f>
+        <v>#REF!</v>
       </c>
       <c r="D93" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F149=0," ",'[1]Complete Route Listing'!F149)</f>
@@ -4970,8 +4970,8 @@
         <v>red</v>
       </c>
       <c r="C94" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D235=0," ",'[1]Complete Route Listing'!D235)</f>
-        <v>6a+</v>
+        <f>IF('[1]Complete Route Listing'!D150=0," ",'[1]Complete Route Listing'!D150)</f>
+        <v>6c+</v>
       </c>
       <c r="D94" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F150=0," ",'[1]Complete Route Listing'!F150)</f>
@@ -4990,8 +4990,8 @@
         <v>black</v>
       </c>
       <c r="C95" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D238=0," ",'[1]Complete Route Listing'!D238)</f>
-        <v>6a+</v>
+        <f>IF('[1]Complete Route Listing'!D151=0," ",'[1]Complete Route Listing'!D151)</f>
+        <v>6a</v>
       </c>
       <c r="D95" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F151=0," ",'[1]Complete Route Listing'!F151)</f>
@@ -5009,9 +5009,9 @@
         <f>IF('[1]Complete Route Listing'!C152=0," ",'[1]Complete Route Listing'!C152)</f>
         <v>green</v>
       </c>
-      <c r="C96" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D63=0," ",'[1]Complete Route Listing'!D63)</f>
-        <v>6a+</v>
+      <c r="C96" s="12">
+        <f>IF('[1]Complete Route Listing'!D152=0," ",'[1]Complete Route Listing'!D152)</f>
+        <v>5</v>
       </c>
       <c r="D96" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F152=0," ",'[1]Complete Route Listing'!F152)</f>
@@ -5029,9 +5029,9 @@
         <f>IF('[1]Complete Route Listing'!C153=0," ",'[1]Complete Route Listing'!C153)</f>
         <v>#REF!</v>
       </c>
-      <c r="C97" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D72=0," ",'[1]Complete Route Listing'!D72)</f>
-        <v>6a+</v>
+      <c r="C97" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D153=0," ",'[1]Complete Route Listing'!D153)</f>
+        <v>#REF!</v>
       </c>
       <c r="D97" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F153=0," ",'[1]Complete Route Listing'!F153)</f>
@@ -5043,10 +5043,7 @@
     <row r="98" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="10"/>
       <c r="B98" s="13"/>
-      <c r="C98" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D78=0," ",'[1]Complete Route Listing'!D78)</f>
-        <v>6a+</v>
-      </c>
+      <c r="C98" s="12"/>
       <c r="D98" s="13"/>
       <c r="E98" s="11"/>
       <c r="F98" s="14"/>
@@ -5060,9 +5057,9 @@
         <f>IF('[1]Complete Route Listing'!C202=0," ",'[1]Complete Route Listing'!C202)</f>
         <v>#REF!</v>
       </c>
-      <c r="C99" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D96=0," ",'[1]Complete Route Listing'!D96)</f>
-        <v>6a+</v>
+      <c r="C99" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D202=0," ",'[1]Complete Route Listing'!D202)</f>
+        <v>#REF!</v>
       </c>
       <c r="D99" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F202=0," ",'[1]Complete Route Listing'!F202)</f>
@@ -5080,9 +5077,9 @@
         <f>IF('[1]Complete Route Listing'!C203=0," ",'[1]Complete Route Listing'!C203)</f>
         <v>#REF!</v>
       </c>
-      <c r="C100" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D158=0," ",'[1]Complete Route Listing'!D158)</f>
-        <v>6a+</v>
+      <c r="C100" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D203=0," ",'[1]Complete Route Listing'!D203)</f>
+        <v>#REF!</v>
       </c>
       <c r="D100" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F203=0," ",'[1]Complete Route Listing'!F203)</f>
@@ -5100,9 +5097,9 @@
         <f>IF('[1]Complete Route Listing'!C204=0," ",'[1]Complete Route Listing'!C204)</f>
         <v>#REF!</v>
       </c>
-      <c r="C101" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D187=0," ",'[1]Complete Route Listing'!D187)</f>
-        <v>6a+</v>
+      <c r="C101" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D204=0," ",'[1]Complete Route Listing'!D204)</f>
+        <v>#REF!</v>
       </c>
       <c r="D101" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F204=0," ",'[1]Complete Route Listing'!F204)</f>
@@ -5120,9 +5117,9 @@
         <f>IF('[1]Complete Route Listing'!C205=0," ",'[1]Complete Route Listing'!C205)</f>
         <v>#REF!</v>
       </c>
-      <c r="C102" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D196=0," ",'[1]Complete Route Listing'!D196)</f>
-        <v>6a+</v>
+      <c r="C102" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D205=0," ",'[1]Complete Route Listing'!D205)</f>
+        <v>#REF!</v>
       </c>
       <c r="D102" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F205=0," ",'[1]Complete Route Listing'!F205)</f>
@@ -5141,7 +5138,7 @@
         <v>red</v>
       </c>
       <c r="C103" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D201=0," ",'[1]Complete Route Listing'!D201)</f>
+        <f>IF('[1]Complete Route Listing'!D210=0," ",'[1]Complete Route Listing'!D210)</f>
         <v>6a+</v>
       </c>
       <c r="D103" s="13" t="str">
@@ -5161,8 +5158,8 @@
         <v>green</v>
       </c>
       <c r="C104" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D256=0," ",'[1]Complete Route Listing'!D256)</f>
-        <v>6a+</v>
+        <f>IF('[1]Complete Route Listing'!D211=0," ",'[1]Complete Route Listing'!D211)</f>
+        <v>7b</v>
       </c>
       <c r="D104" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F211=0," ",'[1]Complete Route Listing'!F211)</f>
@@ -5181,8 +5178,8 @@
         <v>pink</v>
       </c>
       <c r="C105" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D258=0," ",'[1]Complete Route Listing'!D258)</f>
-        <v>6a+</v>
+        <f>IF('[1]Complete Route Listing'!D212=0," ",'[1]Complete Route Listing'!D212)</f>
+        <v>6c+</v>
       </c>
       <c r="D105" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F212=0," ",'[1]Complete Route Listing'!F212)</f>
@@ -5200,9 +5197,9 @@
         <f>IF('[1]Complete Route Listing'!C213=0," ",'[1]Complete Route Listing'!C213)</f>
         <v>#REF!</v>
       </c>
-      <c r="C106" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D270=0," ",'[1]Complete Route Listing'!D270)</f>
-        <v>6a+</v>
+      <c r="C106" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D213=0," ",'[1]Complete Route Listing'!D213)</f>
+        <v>#REF!</v>
       </c>
       <c r="D106" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F213=0," ",'[1]Complete Route Listing'!F213)</f>
@@ -5221,8 +5218,8 @@
         <v>yellow</v>
       </c>
       <c r="C107" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D107=0," ",'[1]Complete Route Listing'!D107)</f>
-        <v>6b</v>
+        <f>IF('[1]Complete Route Listing'!D214=0," ",'[1]Complete Route Listing'!D214)</f>
+        <v>8a+</v>
       </c>
       <c r="D107" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F214=0," ",'[1]Complete Route Listing'!F214)</f>
@@ -5241,8 +5238,8 @@
         <v>orange</v>
       </c>
       <c r="C108" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D114=0," ",'[1]Complete Route Listing'!D114)</f>
-        <v>6b</v>
+        <f>IF('[1]Complete Route Listing'!D215=0," ",'[1]Complete Route Listing'!D215)</f>
+        <v>6c</v>
       </c>
       <c r="D108" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F215=0," ",'[1]Complete Route Listing'!F215)</f>
@@ -5261,8 +5258,8 @@
         <v>white</v>
       </c>
       <c r="C109" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D144=0," ",'[1]Complete Route Listing'!D144)</f>
-        <v>6b</v>
+        <f>IF('[1]Complete Route Listing'!D216=0," ",'[1]Complete Route Listing'!D216)</f>
+        <v>7b+</v>
       </c>
       <c r="D109" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F216=0," ",'[1]Complete Route Listing'!F216)</f>
@@ -5280,9 +5277,9 @@
         <f>IF('[1]Complete Route Listing'!C217=0," ",'[1]Complete Route Listing'!C217)</f>
         <v>#REF!</v>
       </c>
-      <c r="C110" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D218=0," ",'[1]Complete Route Listing'!D218)</f>
-        <v>6b</v>
+      <c r="C110" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D217=0," ",'[1]Complete Route Listing'!D217)</f>
+        <v>#REF!</v>
       </c>
       <c r="D110" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F217=0," ",'[1]Complete Route Listing'!F217)</f>
@@ -5301,7 +5298,7 @@
         <v>blue</v>
       </c>
       <c r="C111" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D227=0," ",'[1]Complete Route Listing'!D227)</f>
+        <f>IF('[1]Complete Route Listing'!D218=0," ",'[1]Complete Route Listing'!D218)</f>
         <v>6b</v>
       </c>
       <c r="D111" s="13" t="str">
@@ -5321,8 +5318,8 @@
         <v>pink</v>
       </c>
       <c r="C112" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D228=0," ",'[1]Complete Route Listing'!D228)</f>
-        <v>6b</v>
+        <f>IF('[1]Complete Route Listing'!D219=0," ",'[1]Complete Route Listing'!D219)</f>
+        <v>6c</v>
       </c>
       <c r="D112" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F219=0," ",'[1]Complete Route Listing'!F219)</f>
@@ -5341,8 +5338,8 @@
         <v>red</v>
       </c>
       <c r="C113" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D234=0," ",'[1]Complete Route Listing'!D234)</f>
-        <v>6b</v>
+        <f>IF('[1]Complete Route Listing'!D220=0," ",'[1]Complete Route Listing'!D220)</f>
+        <v>7c</v>
       </c>
       <c r="D113" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F220=0," ",'[1]Complete Route Listing'!F220)</f>
@@ -5360,9 +5357,9 @@
         <f>IF('[1]Complete Route Listing'!C221=0," ",'[1]Complete Route Listing'!C221)</f>
         <v>#REF!</v>
       </c>
-      <c r="C114" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D239=0," ",'[1]Complete Route Listing'!D239)</f>
-        <v>6b</v>
+      <c r="C114" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D221=0," ",'[1]Complete Route Listing'!D221)</f>
+        <v>#REF!</v>
       </c>
       <c r="D114" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F221=0," ",'[1]Complete Route Listing'!F221)</f>
@@ -5381,8 +5378,8 @@
         <v>purple</v>
       </c>
       <c r="C115" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D251=0," ",'[1]Complete Route Listing'!D251)</f>
-        <v>6b</v>
+        <f>IF('[1]Complete Route Listing'!D222=0," ",'[1]Complete Route Listing'!D222)</f>
+        <v>8a</v>
       </c>
       <c r="D115" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F222=0," ",'[1]Complete Route Listing'!F222)</f>
@@ -5401,8 +5398,8 @@
         <v>yellow</v>
       </c>
       <c r="C116" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D71=0," ",'[1]Complete Route Listing'!D71)</f>
-        <v>6b</v>
+        <f>IF('[1]Complete Route Listing'!D223=0," ",'[1]Complete Route Listing'!D223)</f>
+        <v>7b</v>
       </c>
       <c r="D116" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F223=0," ",'[1]Complete Route Listing'!F223)</f>
@@ -5421,8 +5418,8 @@
         <v>green</v>
       </c>
       <c r="C117" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D90=0," ",'[1]Complete Route Listing'!D90)</f>
-        <v>6b</v>
+        <f>IF('[1]Complete Route Listing'!D224=0," ",'[1]Complete Route Listing'!D224)</f>
+        <v>6c</v>
       </c>
       <c r="D117" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F224=0," ",'[1]Complete Route Listing'!F224)</f>
@@ -5440,9 +5437,9 @@
         <f>IF('[1]Complete Route Listing'!C225=0," ",'[1]Complete Route Listing'!C225)</f>
         <v>#REF!</v>
       </c>
-      <c r="C118" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D100=0," ",'[1]Complete Route Listing'!D100)</f>
-        <v>6b</v>
+      <c r="C118" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D225=0," ",'[1]Complete Route Listing'!D225)</f>
+        <v>#REF!</v>
       </c>
       <c r="D118" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F225=0," ",'[1]Complete Route Listing'!F225)</f>
@@ -5461,8 +5458,8 @@
         <v>blue</v>
       </c>
       <c r="C119" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D101=0," ",'[1]Complete Route Listing'!D101)</f>
-        <v>6b</v>
+        <f>IF('[1]Complete Route Listing'!D226=0," ",'[1]Complete Route Listing'!D226)</f>
+        <v>6c</v>
       </c>
       <c r="D119" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F226=0," ",'[1]Complete Route Listing'!F226)</f>
@@ -5481,7 +5478,7 @@
         <v>red</v>
       </c>
       <c r="C120" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D159=0," ",'[1]Complete Route Listing'!D159)</f>
+        <f>IF('[1]Complete Route Listing'!D227=0," ",'[1]Complete Route Listing'!D227)</f>
         <v>6b</v>
       </c>
       <c r="D120" s="13" t="str">
@@ -5501,7 +5498,7 @@
         <v>orange</v>
       </c>
       <c r="C121" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D175=0," ",'[1]Complete Route Listing'!D175)</f>
+        <f>IF('[1]Complete Route Listing'!D228=0," ",'[1]Complete Route Listing'!D228)</f>
         <v>6b</v>
       </c>
       <c r="D121" s="13" t="str">
@@ -5520,9 +5517,9 @@
         <f>IF('[1]Complete Route Listing'!C229=0," ",'[1]Complete Route Listing'!C229)</f>
         <v>#REF!</v>
       </c>
-      <c r="C122" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D176=0," ",'[1]Complete Route Listing'!D176)</f>
-        <v>6b</v>
+      <c r="C122" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D229=0," ",'[1]Complete Route Listing'!D229)</f>
+        <v>#REF!</v>
       </c>
       <c r="D122" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F229=0," ",'[1]Complete Route Listing'!F229)</f>
@@ -5541,8 +5538,8 @@
         <v>pink</v>
       </c>
       <c r="C123" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D199=0," ",'[1]Complete Route Listing'!D199)</f>
-        <v>6b</v>
+        <f>IF('[1]Complete Route Listing'!D230=0," ",'[1]Complete Route Listing'!D230)</f>
+        <v>6a+</v>
       </c>
       <c r="D123" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F230=0," ",'[1]Complete Route Listing'!F230)</f>
@@ -5560,9 +5557,9 @@
         <f>IF('[1]Complete Route Listing'!C231=0," ",'[1]Complete Route Listing'!C231)</f>
         <v>#REF!</v>
       </c>
-      <c r="C124" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D262=0," ",'[1]Complete Route Listing'!D262)</f>
-        <v>6b</v>
+      <c r="C124" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D231=0," ",'[1]Complete Route Listing'!D231)</f>
+        <v>#REF!</v>
       </c>
       <c r="D124" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F231=0," ",'[1]Complete Route Listing'!F231)</f>
@@ -5580,9 +5577,9 @@
         <f>IF('[1]Complete Route Listing'!C232=0," ",'[1]Complete Route Listing'!C232)</f>
         <v>#REF!</v>
       </c>
-      <c r="C125" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D266=0," ",'[1]Complete Route Listing'!D266)</f>
-        <v>6b</v>
+      <c r="C125" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D232=0," ",'[1]Complete Route Listing'!D232)</f>
+        <v>#REF!</v>
       </c>
       <c r="D125" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F232=0," ",'[1]Complete Route Listing'!F232)</f>
@@ -5600,9 +5597,9 @@
         <f>IF('[1]Complete Route Listing'!C233=0," ",'[1]Complete Route Listing'!C233)</f>
         <v>#REF!</v>
       </c>
-      <c r="C126" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D267=0," ",'[1]Complete Route Listing'!D267)</f>
-        <v>6b</v>
+      <c r="C126" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D233=0," ",'[1]Complete Route Listing'!D233)</f>
+        <v>#REF!</v>
       </c>
       <c r="D126" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F233=0," ",'[1]Complete Route Listing'!F233)</f>
@@ -5621,7 +5618,7 @@
         <v>purple</v>
       </c>
       <c r="C127" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D287=0," ",'[1]Complete Route Listing'!D287)</f>
+        <f>IF('[1]Complete Route Listing'!D234=0," ",'[1]Complete Route Listing'!D234)</f>
         <v>6b</v>
       </c>
       <c r="D127" s="13" t="str">
@@ -5641,8 +5638,8 @@
         <v>red</v>
       </c>
       <c r="C128" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D294=0," ",'[1]Complete Route Listing'!D294)</f>
-        <v>6b</v>
+        <f>IF('[1]Complete Route Listing'!D235=0," ",'[1]Complete Route Listing'!D235)</f>
+        <v>6a+</v>
       </c>
       <c r="D128" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F235=0," ",'[1]Complete Route Listing'!F235)</f>
@@ -5660,9 +5657,9 @@
         <f>IF('[1]Complete Route Listing'!C236=0," ",'[1]Complete Route Listing'!C236)</f>
         <v>#REF!</v>
       </c>
-      <c r="C129" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D51=0," ",'[1]Complete Route Listing'!D51)</f>
-        <v>6b+</v>
+      <c r="C129" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D236=0," ",'[1]Complete Route Listing'!D236)</f>
+        <v>#REF!</v>
       </c>
       <c r="D129" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F236=0," ",'[1]Complete Route Listing'!F236)</f>
@@ -5680,9 +5677,9 @@
         <f>IF('[1]Complete Route Listing'!C237=0," ",'[1]Complete Route Listing'!C237)</f>
         <v>#REF!</v>
       </c>
-      <c r="C130" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D110=0," ",'[1]Complete Route Listing'!D110)</f>
-        <v>6b+</v>
+      <c r="C130" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D237=0," ",'[1]Complete Route Listing'!D237)</f>
+        <v>#REF!</v>
       </c>
       <c r="D130" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F237=0," ",'[1]Complete Route Listing'!F237)</f>
@@ -5701,8 +5698,8 @@
         <v>flo yellow</v>
       </c>
       <c r="C131" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D119=0," ",'[1]Complete Route Listing'!D119)</f>
-        <v>6b+</v>
+        <f>IF('[1]Complete Route Listing'!D238=0," ",'[1]Complete Route Listing'!D238)</f>
+        <v>6a+</v>
       </c>
       <c r="D131" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F238=0," ",'[1]Complete Route Listing'!F238)</f>
@@ -5721,8 +5718,8 @@
         <v>pink</v>
       </c>
       <c r="C132" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D79=0," ",'[1]Complete Route Listing'!D79)</f>
-        <v>6b+</v>
+        <f>IF('[1]Complete Route Listing'!D239=0," ",'[1]Complete Route Listing'!D239)</f>
+        <v>6b</v>
       </c>
       <c r="D132" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F239=0," ",'[1]Complete Route Listing'!F239)</f>
@@ -5741,8 +5738,8 @@
         <v>white</v>
       </c>
       <c r="C133" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D87=0," ",'[1]Complete Route Listing'!D87)</f>
-        <v>6b+</v>
+        <f>IF('[1]Complete Route Listing'!D240=0," ",'[1]Complete Route Listing'!D240)</f>
+        <v>5+</v>
       </c>
       <c r="D133" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F240=0," ",'[1]Complete Route Listing'!F240)</f>
@@ -5761,8 +5758,8 @@
         <v>blue</v>
       </c>
       <c r="C134" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D98=0," ",'[1]Complete Route Listing'!D98)</f>
-        <v>6b+</v>
+        <f>IF('[1]Complete Route Listing'!D241=0," ",'[1]Complete Route Listing'!D241)</f>
+        <v>4+</v>
       </c>
       <c r="D134" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F241=0," ",'[1]Complete Route Listing'!F241)</f>
@@ -5781,8 +5778,8 @@
         <v>green</v>
       </c>
       <c r="C135" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D168=0," ",'[1]Complete Route Listing'!D168)</f>
-        <v>6b+</v>
+        <f>IF('[1]Complete Route Listing'!D242=0," ",'[1]Complete Route Listing'!D242)</f>
+        <v>6a</v>
       </c>
       <c r="D135" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F242=0," ",'[1]Complete Route Listing'!F242)</f>
@@ -5801,8 +5798,8 @@
         <v>red</v>
       </c>
       <c r="C136" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D182=0," ",'[1]Complete Route Listing'!D182)</f>
-        <v>6b+</v>
+        <f>IF('[1]Complete Route Listing'!D243=0," ",'[1]Complete Route Listing'!D243)</f>
+        <v>6c+</v>
       </c>
       <c r="D136" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F243=0," ",'[1]Complete Route Listing'!F243)</f>
@@ -5820,9 +5817,9 @@
         <f>IF('[1]Complete Route Listing'!C244=0," ",'[1]Complete Route Listing'!C244)</f>
         <v>#REF!</v>
       </c>
-      <c r="C137" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D194=0," ",'[1]Complete Route Listing'!D194)</f>
-        <v>6b+</v>
+      <c r="C137" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D244=0," ",'[1]Complete Route Listing'!D244)</f>
+        <v>#REF!</v>
       </c>
       <c r="D137" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F244=0," ",'[1]Complete Route Listing'!F244)</f>
@@ -5840,9 +5837,9 @@
         <f>IF('[1]Complete Route Listing'!C245=0," ",'[1]Complete Route Listing'!C245)</f>
         <v>#REF!</v>
       </c>
-      <c r="C138" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D106=0," ",'[1]Complete Route Listing'!D106)</f>
-        <v>6c</v>
+      <c r="C138" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D245=0," ",'[1]Complete Route Listing'!D245)</f>
+        <v>#REF!</v>
       </c>
       <c r="D138" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F245=0," ",'[1]Complete Route Listing'!F245)</f>
@@ -5861,8 +5858,8 @@
         <v>orange</v>
       </c>
       <c r="C139" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D108=0," ",'[1]Complete Route Listing'!D108)</f>
-        <v>6c</v>
+        <f>IF('[1]Complete Route Listing'!D246=0," ",'[1]Complete Route Listing'!D246)</f>
+        <v>7a+</v>
       </c>
       <c r="D139" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F246=0," ",'[1]Complete Route Listing'!F246)</f>
@@ -5881,8 +5878,8 @@
         <v>blue</v>
       </c>
       <c r="C140" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D132=0," ",'[1]Complete Route Listing'!D132)</f>
-        <v>6c</v>
+        <f>IF('[1]Complete Route Listing'!D247=0," ",'[1]Complete Route Listing'!D247)</f>
+        <v>7a</v>
       </c>
       <c r="D140" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F247=0," ",'[1]Complete Route Listing'!F247)</f>
@@ -5900,9 +5897,9 @@
         <f>IF('[1]Complete Route Listing'!C248=0," ",'[1]Complete Route Listing'!C248)</f>
         <v>yellow</v>
       </c>
-      <c r="C141" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D215=0," ",'[1]Complete Route Listing'!D215)</f>
-        <v>6c</v>
+      <c r="C141" s="12">
+        <f>IF('[1]Complete Route Listing'!D248=0," ",'[1]Complete Route Listing'!D248)</f>
+        <v>5</v>
       </c>
       <c r="D141" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F248=0," ",'[1]Complete Route Listing'!F248)</f>
@@ -5920,9 +5917,9 @@
         <f>IF('[1]Complete Route Listing'!C249=0," ",'[1]Complete Route Listing'!C249)</f>
         <v>#REF!</v>
       </c>
-      <c r="C142" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D219=0," ",'[1]Complete Route Listing'!D219)</f>
-        <v>6c</v>
+      <c r="C142" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D249=0," ",'[1]Complete Route Listing'!D249)</f>
+        <v>#REF!</v>
       </c>
       <c r="D142" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F249=0," ",'[1]Complete Route Listing'!F249)</f>
@@ -5941,8 +5938,8 @@
         <v>white</v>
       </c>
       <c r="C143" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D224=0," ",'[1]Complete Route Listing'!D224)</f>
-        <v>6c</v>
+        <f>IF('[1]Complete Route Listing'!D250=0," ",'[1]Complete Route Listing'!D250)</f>
+        <v>4+</v>
       </c>
       <c r="D143" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F250=0," ",'[1]Complete Route Listing'!F250)</f>
@@ -5961,8 +5958,8 @@
         <v>yellow</v>
       </c>
       <c r="C144" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D226=0," ",'[1]Complete Route Listing'!D226)</f>
-        <v>6c</v>
+        <f>IF('[1]Complete Route Listing'!D251=0," ",'[1]Complete Route Listing'!D251)</f>
+        <v>6b</v>
       </c>
       <c r="D144" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F251=0," ",'[1]Complete Route Listing'!F251)</f>
@@ -5980,9 +5977,9 @@
         <f>IF('[1]Complete Route Listing'!C252=0," ",'[1]Complete Route Listing'!C252)</f>
         <v>#REF!</v>
       </c>
-      <c r="C145" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D59=0," ",'[1]Complete Route Listing'!D59)</f>
-        <v>6C</v>
+      <c r="C145" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D252=0," ",'[1]Complete Route Listing'!D252)</f>
+        <v>#REF!</v>
       </c>
       <c r="D145" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F252=0," ",'[1]Complete Route Listing'!F252)</f>
@@ -6001,8 +5998,8 @@
         <v>yellow</v>
       </c>
       <c r="C146" s="7" t="str">
-        <f>IF('[1]Complete Route Listing'!D82=0," ",'[1]Complete Route Listing'!D82)</f>
-        <v>6c</v>
+        <f>IF('[1]Complete Route Listing'!D58=0," ",'[1]Complete Route Listing'!D58)</f>
+        <v>6a</v>
       </c>
       <c r="D146" s="8" t="str">
         <f>IF('[1]Complete Route Listing'!F58=0," ",'[1]Complete Route Listing'!F58)</f>
@@ -6027,8 +6024,8 @@
         <v>white</v>
       </c>
       <c r="C147" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D99=0," ",'[1]Complete Route Listing'!D99)</f>
-        <v>6c</v>
+        <f>IF('[1]Complete Route Listing'!D59=0," ",'[1]Complete Route Listing'!D59)</f>
+        <v>6C</v>
       </c>
       <c r="D147" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F59=0," ",'[1]Complete Route Listing'!F59)</f>
@@ -6052,9 +6049,9 @@
         <f>IF('[1]Complete Route Listing'!C60=0," ",'[1]Complete Route Listing'!C60)</f>
         <v>#REF!</v>
       </c>
-      <c r="C148" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D154=0," ",'[1]Complete Route Listing'!D154)</f>
-        <v>6c</v>
+      <c r="C148" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D60=0," ",'[1]Complete Route Listing'!D60)</f>
+        <v>#REF!</v>
       </c>
       <c r="D148" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F60=0," ",'[1]Complete Route Listing'!F60)</f>
@@ -6072,9 +6069,9 @@
         <f>IF('[1]Complete Route Listing'!C61=0," ",'[1]Complete Route Listing'!C61)</f>
         <v>#REF!</v>
       </c>
-      <c r="C149" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D164=0," ",'[1]Complete Route Listing'!D164)</f>
-        <v>6c</v>
+      <c r="C149" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D61=0," ",'[1]Complete Route Listing'!D61)</f>
+        <v>#REF!</v>
       </c>
       <c r="D149" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F61=0," ",'[1]Complete Route Listing'!F61)</f>
@@ -6092,9 +6089,9 @@
         <f>IF('[1]Complete Route Listing'!C62=0," ",'[1]Complete Route Listing'!C62)</f>
         <v>red</v>
       </c>
-      <c r="C150" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D200=0," ",'[1]Complete Route Listing'!D200)</f>
-        <v>6c</v>
+      <c r="C150" s="12">
+        <f>IF('[1]Complete Route Listing'!D62=0," ",'[1]Complete Route Listing'!D62)</f>
+        <v>5</v>
       </c>
       <c r="D150" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F62=0," ",'[1]Complete Route Listing'!F62)</f>
@@ -6113,8 +6110,8 @@
         <v>blue</v>
       </c>
       <c r="C151" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D254=0," ",'[1]Complete Route Listing'!D254)</f>
-        <v>6c</v>
+        <f>IF('[1]Complete Route Listing'!D63=0," ",'[1]Complete Route Listing'!D63)</f>
+        <v>6a+</v>
       </c>
       <c r="D151" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F63=0," ",'[1]Complete Route Listing'!F63)</f>
@@ -6132,9 +6129,9 @@
         <f>IF('[1]Complete Route Listing'!C64=0," ",'[1]Complete Route Listing'!C64)</f>
         <v>#REF!</v>
       </c>
-      <c r="C152" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D263=0," ",'[1]Complete Route Listing'!D263)</f>
-        <v>6c</v>
+      <c r="C152" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D64=0," ",'[1]Complete Route Listing'!D64)</f>
+        <v>#REF!</v>
       </c>
       <c r="D152" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F64=0," ",'[1]Complete Route Listing'!F64)</f>
@@ -6152,9 +6149,9 @@
         <f>IF('[1]Complete Route Listing'!C65=0," ",'[1]Complete Route Listing'!C65)</f>
         <v>#REF!</v>
       </c>
-      <c r="C153" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D279=0," ",'[1]Complete Route Listing'!D279)</f>
-        <v>6c</v>
+      <c r="C153" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D65=0," ",'[1]Complete Route Listing'!D65)</f>
+        <v>#REF!</v>
       </c>
       <c r="D153" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F65=0," ",'[1]Complete Route Listing'!F65)</f>
@@ -6172,9 +6169,9 @@
         <f>IF('[1]Complete Route Listing'!C66=0," ",'[1]Complete Route Listing'!C66)</f>
         <v>purple</v>
       </c>
-      <c r="C154" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D139=0," ",'[1]Complete Route Listing'!D139)</f>
-        <v>6c+</v>
+      <c r="C154" s="12">
+        <f>IF('[1]Complete Route Listing'!D66=0," ",'[1]Complete Route Listing'!D66)</f>
+        <v>4</v>
       </c>
       <c r="D154" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F66=0," ",'[1]Complete Route Listing'!F66)</f>
@@ -6193,8 +6190,8 @@
         <v>green</v>
       </c>
       <c r="C155" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D150=0," ",'[1]Complete Route Listing'!D150)</f>
-        <v>6c+</v>
+        <f>IF('[1]Complete Route Listing'!D67=0," ",'[1]Complete Route Listing'!D67)</f>
+        <v>6a</v>
       </c>
       <c r="D155" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F67=0," ",'[1]Complete Route Listing'!F67)</f>
@@ -6212,9 +6209,9 @@
         <f>IF('[1]Complete Route Listing'!C68=0," ",'[1]Complete Route Listing'!C68)</f>
         <v>#REF!</v>
       </c>
-      <c r="C156" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D212=0," ",'[1]Complete Route Listing'!D212)</f>
-        <v>6c+</v>
+      <c r="C156" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D68=0," ",'[1]Complete Route Listing'!D68)</f>
+        <v>#REF!</v>
       </c>
       <c r="D156" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F68=0," ",'[1]Complete Route Listing'!F68)</f>
@@ -6232,9 +6229,9 @@
         <f>IF('[1]Complete Route Listing'!C69=0," ",'[1]Complete Route Listing'!C69)</f>
         <v>#REF!</v>
       </c>
-      <c r="C157" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D243=0," ",'[1]Complete Route Listing'!D243)</f>
-        <v>6c+</v>
+      <c r="C157" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D69=0," ",'[1]Complete Route Listing'!D69)</f>
+        <v>#REF!</v>
       </c>
       <c r="D157" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F69=0," ",'[1]Complete Route Listing'!F69)</f>
@@ -6252,9 +6249,9 @@
         <f>IF('[1]Complete Route Listing'!C70=0," ",'[1]Complete Route Listing'!C70)</f>
         <v>orange</v>
       </c>
-      <c r="C158" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D94=0," ",'[1]Complete Route Listing'!D94)</f>
-        <v>6c+</v>
+      <c r="C158" s="12">
+        <f>IF('[1]Complete Route Listing'!D70=0," ",'[1]Complete Route Listing'!D70)</f>
+        <v>5</v>
       </c>
       <c r="D158" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F70=0," ",'[1]Complete Route Listing'!F70)</f>
@@ -6276,8 +6273,8 @@
         <v>green</v>
       </c>
       <c r="C159" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D179=0," ",'[1]Complete Route Listing'!D179)</f>
-        <v>6c+</v>
+        <f>IF('[1]Complete Route Listing'!D71=0," ",'[1]Complete Route Listing'!D71)</f>
+        <v>6b</v>
       </c>
       <c r="D159" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F71=0," ",'[1]Complete Route Listing'!F71)</f>
@@ -6299,8 +6296,8 @@
         <v>black</v>
       </c>
       <c r="C160" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D190=0," ",'[1]Complete Route Listing'!D190)</f>
-        <v>6c+</v>
+        <f>IF('[1]Complete Route Listing'!D72=0," ",'[1]Complete Route Listing'!D72)</f>
+        <v>6a+</v>
       </c>
       <c r="D160" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F72=0," ",'[1]Complete Route Listing'!F72)</f>
@@ -6321,9 +6318,9 @@
         <f>IF('[1]Complete Route Listing'!C73=0," ",'[1]Complete Route Listing'!C73)</f>
         <v>#REF!</v>
       </c>
-      <c r="C161" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D255=0," ",'[1]Complete Route Listing'!D255)</f>
-        <v>6c+</v>
+      <c r="C161" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D73=0," ",'[1]Complete Route Listing'!D73)</f>
+        <v>#REF!</v>
       </c>
       <c r="D161" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F73=0," ",'[1]Complete Route Listing'!F73)</f>
@@ -6344,9 +6341,9 @@
         <f>IF('[1]Complete Route Listing'!C74=0," ",'[1]Complete Route Listing'!C74)</f>
         <v>white</v>
       </c>
-      <c r="C162" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D271=0," ",'[1]Complete Route Listing'!D271)</f>
-        <v>6c+</v>
+      <c r="C162" s="12">
+        <f>IF('[1]Complete Route Listing'!D74=0," ",'[1]Complete Route Listing'!D74)</f>
+        <v>5</v>
       </c>
       <c r="D162" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F74=0," ",'[1]Complete Route Listing'!F74)</f>
@@ -6367,9 +6364,9 @@
         <f>IF('[1]Complete Route Listing'!C75=0," ",'[1]Complete Route Listing'!C75)</f>
         <v>yellow</v>
       </c>
-      <c r="C163" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D128=0," ",'[1]Complete Route Listing'!D128)</f>
-        <v>7a</v>
+      <c r="C163" s="12">
+        <f>IF('[1]Complete Route Listing'!D75=0," ",'[1]Complete Route Listing'!D75)</f>
+        <v>4</v>
       </c>
       <c r="D163" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F75=0," ",'[1]Complete Route Listing'!F75)</f>
@@ -6391,8 +6388,8 @@
         <v>blue</v>
       </c>
       <c r="C164" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D147=0," ",'[1]Complete Route Listing'!D147)</f>
-        <v>7a</v>
+        <f>IF('[1]Complete Route Listing'!D76=0," ",'[1]Complete Route Listing'!D76)</f>
+        <v>5+</v>
       </c>
       <c r="D164" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F76=0," ",'[1]Complete Route Listing'!F76)</f>
@@ -6413,9 +6410,9 @@
         <f>IF('[1]Complete Route Listing'!C77=0," ",'[1]Complete Route Listing'!C77)</f>
         <v>#REF!</v>
       </c>
-      <c r="C165" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D247=0," ",'[1]Complete Route Listing'!D247)</f>
-        <v>7a</v>
+      <c r="C165" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D77=0," ",'[1]Complete Route Listing'!D77)</f>
+        <v>#REF!</v>
       </c>
       <c r="D165" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F77=0," ",'[1]Complete Route Listing'!F77)</f>
@@ -6437,8 +6434,8 @@
         <v>purple</v>
       </c>
       <c r="C166" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D103=0," ",'[1]Complete Route Listing'!D103)</f>
-        <v>7a</v>
+        <f>IF('[1]Complete Route Listing'!D78=0," ",'[1]Complete Route Listing'!D78)</f>
+        <v>6a+</v>
       </c>
       <c r="D166" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F78=0," ",'[1]Complete Route Listing'!F78)</f>
@@ -6460,8 +6457,8 @@
         <v>red</v>
       </c>
       <c r="C167" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D160=0," ",'[1]Complete Route Listing'!D160)</f>
-        <v>7a</v>
+        <f>IF('[1]Complete Route Listing'!D79=0," ",'[1]Complete Route Listing'!D79)</f>
+        <v>6b+</v>
       </c>
       <c r="D167" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F79=0," ",'[1]Complete Route Listing'!F79)</f>
@@ -6482,9 +6479,9 @@
         <f>IF('[1]Complete Route Listing'!C80=0," ",'[1]Complete Route Listing'!C80)</f>
         <v>black</v>
       </c>
-      <c r="C168" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D171=0," ",'[1]Complete Route Listing'!D171)</f>
-        <v>7a</v>
+      <c r="C168" s="12">
+        <f>IF('[1]Complete Route Listing'!D80=0," ",'[1]Complete Route Listing'!D80)</f>
+        <v>5</v>
       </c>
       <c r="D168" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F80=0," ",'[1]Complete Route Listing'!F80)</f>
@@ -6505,9 +6502,9 @@
         <f>IF('[1]Complete Route Listing'!C81=0," ",'[1]Complete Route Listing'!C81)</f>
         <v>#REF!</v>
       </c>
-      <c r="C169" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D174=0," ",'[1]Complete Route Listing'!D174)</f>
-        <v>7a</v>
+      <c r="C169" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D81=0," ",'[1]Complete Route Listing'!D81)</f>
+        <v>#REF!</v>
       </c>
       <c r="D169" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F81=0," ",'[1]Complete Route Listing'!F81)</f>
@@ -6529,8 +6526,8 @@
         <v>pink</v>
       </c>
       <c r="C170" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D122=0," ",'[1]Complete Route Listing'!D122)</f>
-        <v>7a+</v>
+        <f>IF('[1]Complete Route Listing'!D82=0," ",'[1]Complete Route Listing'!D82)</f>
+        <v>6c</v>
       </c>
       <c r="D170" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F82=0," ",'[1]Complete Route Listing'!F82)</f>
@@ -6551,9 +6548,9 @@
         <f>IF('[1]Complete Route Listing'!C83=0," ",'[1]Complete Route Listing'!C83)</f>
         <v>yellow</v>
       </c>
-      <c r="C171" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D246=0," ",'[1]Complete Route Listing'!D246)</f>
-        <v>7a+</v>
+      <c r="C171" s="12">
+        <f>IF('[1]Complete Route Listing'!D83=0," ",'[1]Complete Route Listing'!D83)</f>
+        <v>5</v>
       </c>
       <c r="D171" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F83=0," ",'[1]Complete Route Listing'!F83)</f>
@@ -6575,8 +6572,8 @@
         <v>green</v>
       </c>
       <c r="C172" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D191=0," ",'[1]Complete Route Listing'!D191)</f>
-        <v>7a+</v>
+        <f>IF('[1]Complete Route Listing'!D84=0," ",'[1]Complete Route Listing'!D84)</f>
+        <v>6a</v>
       </c>
       <c r="D172" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F84=0," ",'[1]Complete Route Listing'!F84)</f>
@@ -6598,8 +6595,8 @@
         <v>red</v>
       </c>
       <c r="C173" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D126=0," ",'[1]Complete Route Listing'!D126)</f>
-        <v>7b</v>
+        <f>IF('[1]Complete Route Listing'!D85=0," ",'[1]Complete Route Listing'!D85)</f>
+        <v>5+</v>
       </c>
       <c r="D173" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F85=0," ",'[1]Complete Route Listing'!F85)</f>
@@ -6621,8 +6618,8 @@
         <v>flo yellow</v>
       </c>
       <c r="C174" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D127=0," ",'[1]Complete Route Listing'!D127)</f>
-        <v>7b</v>
+        <f>IF('[1]Complete Route Listing'!D86=0," ",'[1]Complete Route Listing'!D86)</f>
+        <v>6a</v>
       </c>
       <c r="D174" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F86=0," ",'[1]Complete Route Listing'!F86)</f>
@@ -6644,8 +6641,8 @@
         <v>red</v>
       </c>
       <c r="C175" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D211=0," ",'[1]Complete Route Listing'!D211)</f>
-        <v>7b</v>
+        <f>IF('[1]Complete Route Listing'!D87=0," ",'[1]Complete Route Listing'!D87)</f>
+        <v>6b+</v>
       </c>
       <c r="D175" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F87=0," ",'[1]Complete Route Listing'!F87)</f>
@@ -6667,8 +6664,8 @@
         <v>green</v>
       </c>
       <c r="C176" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D223=0," ",'[1]Complete Route Listing'!D223)</f>
-        <v>7b</v>
+        <f>IF('[1]Complete Route Listing'!D88=0," ",'[1]Complete Route Listing'!D88)</f>
+        <v>5+</v>
       </c>
       <c r="D176" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F88=0," ",'[1]Complete Route Listing'!F88)</f>
@@ -6689,9 +6686,9 @@
         <f>IF('[1]Complete Route Listing'!C89=0," ",'[1]Complete Route Listing'!C89)</f>
         <v>#REF!</v>
       </c>
-      <c r="C177" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D155=0," ",'[1]Complete Route Listing'!D155)</f>
-        <v>7b</v>
+      <c r="C177" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D89=0," ",'[1]Complete Route Listing'!D89)</f>
+        <v>#REF!</v>
       </c>
       <c r="D177" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F89=0," ",'[1]Complete Route Listing'!F89)</f>
@@ -6713,8 +6710,8 @@
         <v>blue</v>
       </c>
       <c r="C178" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D130=0," ",'[1]Complete Route Listing'!D130)</f>
-        <v>7b+</v>
+        <f>IF('[1]Complete Route Listing'!D90=0," ",'[1]Complete Route Listing'!D90)</f>
+        <v>6b</v>
       </c>
       <c r="D178" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F90=0," ",'[1]Complete Route Listing'!F90)</f>
@@ -6736,8 +6733,8 @@
         <v>pink</v>
       </c>
       <c r="C179" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D143=0," ",'[1]Complete Route Listing'!D143)</f>
-        <v>7b+</v>
+        <f>IF('[1]Complete Route Listing'!D91=0," ",'[1]Complete Route Listing'!D91)</f>
+        <v>5+</v>
       </c>
       <c r="D179" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F91=0," ",'[1]Complete Route Listing'!F91)</f>
@@ -6759,8 +6756,8 @@
         <v>orange</v>
       </c>
       <c r="C180" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D216=0," ",'[1]Complete Route Listing'!D216)</f>
-        <v>7b+</v>
+        <f>IF('[1]Complete Route Listing'!D92=0," ",'[1]Complete Route Listing'!D92)</f>
+        <v>4+</v>
       </c>
       <c r="D180" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F92=0," ",'[1]Complete Route Listing'!F92)</f>
@@ -6781,9 +6778,9 @@
         <f>IF('[1]Complete Route Listing'!C93=0," ",'[1]Complete Route Listing'!C93)</f>
         <v>#REF!</v>
       </c>
-      <c r="C181" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D170=0," ",'[1]Complete Route Listing'!D170)</f>
-        <v>7b+</v>
+      <c r="C181" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D93=0," ",'[1]Complete Route Listing'!D93)</f>
+        <v>#REF!</v>
       </c>
       <c r="D181" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F93=0," ",'[1]Complete Route Listing'!F93)</f>
@@ -6805,8 +6802,8 @@
         <v>black</v>
       </c>
       <c r="C182" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D146=0," ",'[1]Complete Route Listing'!D146)</f>
-        <v>7c</v>
+        <f>IF('[1]Complete Route Listing'!D94=0," ",'[1]Complete Route Listing'!D94)</f>
+        <v>6c+</v>
       </c>
       <c r="D182" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F94=0," ",'[1]Complete Route Listing'!F94)</f>
@@ -6828,8 +6825,8 @@
         <v>white</v>
       </c>
       <c r="C183" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D220=0," ",'[1]Complete Route Listing'!D220)</f>
-        <v>7c</v>
+        <f>IF('[1]Complete Route Listing'!D95=0," ",'[1]Complete Route Listing'!D95)</f>
+        <v>6a</v>
       </c>
       <c r="D183" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F95=0," ",'[1]Complete Route Listing'!F95)</f>
@@ -6851,8 +6848,8 @@
         <v>red</v>
       </c>
       <c r="C184" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D163=0," ",'[1]Complete Route Listing'!D163)</f>
-        <v>7c</v>
+        <f>IF('[1]Complete Route Listing'!D96=0," ",'[1]Complete Route Listing'!D96)</f>
+        <v>6a+</v>
       </c>
       <c r="D184" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F96=0," ",'[1]Complete Route Listing'!F96)</f>
@@ -6873,9 +6870,9 @@
         <f>IF('[1]Complete Route Listing'!C97=0," ",'[1]Complete Route Listing'!C97)</f>
         <v>#REF!</v>
       </c>
-      <c r="C185" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D162=0," ",'[1]Complete Route Listing'!D162)</f>
-        <v>7c+</v>
+      <c r="C185" s="12" t="e">
+        <f>IF('[1]Complete Route Listing'!D97=0," ",'[1]Complete Route Listing'!D97)</f>
+        <v>#REF!</v>
       </c>
       <c r="D185" s="13" t="e">
         <f>IF('[1]Complete Route Listing'!F97=0," ",'[1]Complete Route Listing'!F97)</f>
@@ -6897,8 +6894,8 @@
         <v>purple</v>
       </c>
       <c r="C186" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D222=0," ",'[1]Complete Route Listing'!D222)</f>
-        <v>8a</v>
+        <f>IF('[1]Complete Route Listing'!D98=0," ",'[1]Complete Route Listing'!D98)</f>
+        <v>6b+</v>
       </c>
       <c r="D186" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F98=0," ",'[1]Complete Route Listing'!F98)</f>
@@ -6920,8 +6917,8 @@
         <v>flo yellow</v>
       </c>
       <c r="C187" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D166=0," ",'[1]Complete Route Listing'!D166)</f>
-        <v>8a</v>
+        <f>IF('[1]Complete Route Listing'!D99=0," ",'[1]Complete Route Listing'!D99)</f>
+        <v>6c</v>
       </c>
       <c r="D187" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F99=0," ",'[1]Complete Route Listing'!F99)</f>
@@ -6943,8 +6940,8 @@
         <v>pink</v>
       </c>
       <c r="C188" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D214=0," ",'[1]Complete Route Listing'!D214)</f>
-        <v>8a+</v>
+        <f>IF('[1]Complete Route Listing'!D100=0," ",'[1]Complete Route Listing'!D100)</f>
+        <v>6b</v>
       </c>
       <c r="D188" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F100=0," ",'[1]Complete Route Listing'!F100)</f>
@@ -6966,8 +6963,8 @@
         <v>blue</v>
       </c>
       <c r="C189" s="12" t="str">
-        <f>IF('[1]Complete Route Listing'!D167=0," ",'[1]Complete Route Listing'!D167)</f>
-        <v>8a+</v>
+        <f>IF('[1]Complete Route Listing'!D101=0," ",'[1]Complete Route Listing'!D101)</f>
+        <v>6b</v>
       </c>
       <c r="D189" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F101=0," ",'[1]Complete Route Listing'!F101)</f>
@@ -6988,9 +6985,9 @@
         <f>IF('[1]Complete Route Listing'!C102=0," ",'[1]Complete Route Listing'!C102)</f>
         <v>red</v>
       </c>
-      <c r="C190" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D12=0," ",'[1]Complete Route Listing'!D12)</f>
-        <v>#REF!</v>
+      <c r="C190" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D102=0," ",'[1]Complete Route Listing'!D102)</f>
+        <v>5+</v>
       </c>
       <c r="D190" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F102=0," ",'[1]Complete Route Listing'!F102)</f>
@@ -7011,9 +7008,9 @@
         <f>IF('[1]Complete Route Listing'!C103=0," ",'[1]Complete Route Listing'!C103)</f>
         <v>green</v>
       </c>
-      <c r="C191" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D13=0," ",'[1]Complete Route Listing'!D13)</f>
-        <v>#REF!</v>
+      <c r="C191" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D103=0," ",'[1]Complete Route Listing'!D103)</f>
+        <v>7a</v>
       </c>
       <c r="D191" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F103=0," ",'[1]Complete Route Listing'!F103)</f>
@@ -7034,9 +7031,9 @@
         <f>IF('[1]Complete Route Listing'!C104=0," ",'[1]Complete Route Listing'!C104)</f>
         <v>black</v>
       </c>
-      <c r="C192" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D16=0," ",'[1]Complete Route Listing'!D16)</f>
-        <v>#REF!</v>
+      <c r="C192" s="12">
+        <f>IF('[1]Complete Route Listing'!D104=0," ",'[1]Complete Route Listing'!D104)</f>
+        <v>4</v>
       </c>
       <c r="D192" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F104=0," ",'[1]Complete Route Listing'!F104)</f>
@@ -7058,7 +7055,7 @@
         <v>#REF!</v>
       </c>
       <c r="C193" s="17" t="e">
-        <f>IF('[1]Complete Route Listing'!D17=0," ",'[1]Complete Route Listing'!D17)</f>
+        <f>IF('[1]Complete Route Listing'!D105=0," ",'[1]Complete Route Listing'!D105)</f>
         <v>#REF!</v>
       </c>
       <c r="D193" s="18" t="e">
@@ -7080,9 +7077,9 @@
         <f>IF('[1]Complete Route Listing'!C154=0," ",'[1]Complete Route Listing'!C154)</f>
         <v>white</v>
       </c>
-      <c r="C194" s="7" t="e">
-        <f>IF('[1]Complete Route Listing'!D20=0," ",'[1]Complete Route Listing'!D20)</f>
-        <v>#REF!</v>
+      <c r="C194" s="7" t="str">
+        <f>IF('[1]Complete Route Listing'!D154=0," ",'[1]Complete Route Listing'!D154)</f>
+        <v>6c</v>
       </c>
       <c r="D194" s="8" t="str">
         <f>IF('[1]Complete Route Listing'!F154=0," ",'[1]Complete Route Listing'!F154)</f>
@@ -7103,9 +7100,9 @@
         <f>IF('[1]Complete Route Listing'!C155=0," ",'[1]Complete Route Listing'!C155)</f>
         <v>pink</v>
       </c>
-      <c r="C195" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D21=0," ",'[1]Complete Route Listing'!D21)</f>
-        <v>#REF!</v>
+      <c r="C195" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D155=0," ",'[1]Complete Route Listing'!D155)</f>
+        <v>7b</v>
       </c>
       <c r="D195" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F155=0," ",'[1]Complete Route Listing'!F155)</f>
@@ -7127,7 +7124,7 @@
         <v>#REF!</v>
       </c>
       <c r="C196" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D24=0," ",'[1]Complete Route Listing'!D24)</f>
+        <f>IF('[1]Complete Route Listing'!D156=0," ",'[1]Complete Route Listing'!D156)</f>
         <v>#REF!</v>
       </c>
       <c r="D196" s="13" t="str">
@@ -7150,7 +7147,7 @@
         <v>#REF!</v>
       </c>
       <c r="C197" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D25=0," ",'[1]Complete Route Listing'!D25)</f>
+        <f>IF('[1]Complete Route Listing'!D157=0," ",'[1]Complete Route Listing'!D157)</f>
         <v>#REF!</v>
       </c>
       <c r="D197" s="13" t="e">
@@ -7172,9 +7169,9 @@
         <f>IF('[1]Complete Route Listing'!C158=0," ",'[1]Complete Route Listing'!C158)</f>
         <v>flo yellow</v>
       </c>
-      <c r="C198" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D28=0," ",'[1]Complete Route Listing'!D28)</f>
-        <v>#REF!</v>
+      <c r="C198" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D158=0," ",'[1]Complete Route Listing'!D158)</f>
+        <v>6a+</v>
       </c>
       <c r="D198" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F158=0," ",'[1]Complete Route Listing'!F158)</f>
@@ -7195,9 +7192,9 @@
         <f>IF('[1]Complete Route Listing'!C159=0," ",'[1]Complete Route Listing'!C159)</f>
         <v>green</v>
       </c>
-      <c r="C199" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D29=0," ",'[1]Complete Route Listing'!D29)</f>
-        <v>#REF!</v>
+      <c r="C199" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D159=0," ",'[1]Complete Route Listing'!D159)</f>
+        <v>6b</v>
       </c>
       <c r="D199" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F159=0," ",'[1]Complete Route Listing'!F159)</f>
@@ -7218,9 +7215,9 @@
         <f>IF('[1]Complete Route Listing'!C160=0," ",'[1]Complete Route Listing'!C160)</f>
         <v>black</v>
       </c>
-      <c r="C200" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D32=0," ",'[1]Complete Route Listing'!D32)</f>
-        <v>#REF!</v>
+      <c r="C200" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D160=0," ",'[1]Complete Route Listing'!D160)</f>
+        <v>7a</v>
       </c>
       <c r="D200" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F160=0," ",'[1]Complete Route Listing'!F160)</f>
@@ -7242,7 +7239,7 @@
         <v>#REF!</v>
       </c>
       <c r="C201" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D33=0," ",'[1]Complete Route Listing'!D33)</f>
+        <f>IF('[1]Complete Route Listing'!D161=0," ",'[1]Complete Route Listing'!D161)</f>
         <v>#REF!</v>
       </c>
       <c r="D201" s="13" t="e">
@@ -7264,9 +7261,9 @@
         <f>IF('[1]Complete Route Listing'!C162=0," ",'[1]Complete Route Listing'!C162)</f>
         <v>orange</v>
       </c>
-      <c r="C202" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D36=0," ",'[1]Complete Route Listing'!D36)</f>
-        <v>#REF!</v>
+      <c r="C202" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D162=0," ",'[1]Complete Route Listing'!D162)</f>
+        <v>7c+</v>
       </c>
       <c r="D202" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F162=0," ",'[1]Complete Route Listing'!F162)</f>
@@ -7287,9 +7284,9 @@
         <f>IF('[1]Complete Route Listing'!C163=0," ",'[1]Complete Route Listing'!C163)</f>
         <v>pink</v>
       </c>
-      <c r="C203" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D37=0," ",'[1]Complete Route Listing'!D37)</f>
-        <v>#REF!</v>
+      <c r="C203" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D163=0," ",'[1]Complete Route Listing'!D163)</f>
+        <v>7c</v>
       </c>
       <c r="D203" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F163=0," ",'[1]Complete Route Listing'!F163)</f>
@@ -7310,9 +7307,9 @@
         <f>IF('[1]Complete Route Listing'!C164=0," ",'[1]Complete Route Listing'!C164)</f>
         <v>red</v>
       </c>
-      <c r="C204" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D40=0," ",'[1]Complete Route Listing'!D40)</f>
-        <v>#REF!</v>
+      <c r="C204" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D164=0," ",'[1]Complete Route Listing'!D164)</f>
+        <v>6c</v>
       </c>
       <c r="D204" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F164=0," ",'[1]Complete Route Listing'!F164)</f>
@@ -7334,7 +7331,7 @@
         <v>#REF!</v>
       </c>
       <c r="C205" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D41=0," ",'[1]Complete Route Listing'!D41)</f>
+        <f>IF('[1]Complete Route Listing'!D165=0," ",'[1]Complete Route Listing'!D165)</f>
         <v>#REF!</v>
       </c>
       <c r="D205" s="13" t="e">
@@ -7356,9 +7353,9 @@
         <f>IF('[1]Complete Route Listing'!C166=0," ",'[1]Complete Route Listing'!C166)</f>
         <v>green</v>
       </c>
-      <c r="C206" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D44=0," ",'[1]Complete Route Listing'!D44)</f>
-        <v>#REF!</v>
+      <c r="C206" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D166=0," ",'[1]Complete Route Listing'!D166)</f>
+        <v>8a</v>
       </c>
       <c r="D206" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F166=0," ",'[1]Complete Route Listing'!F166)</f>
@@ -7379,9 +7376,9 @@
         <f>IF('[1]Complete Route Listing'!C167=0," ",'[1]Complete Route Listing'!C167)</f>
         <v>white</v>
       </c>
-      <c r="C207" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D45=0," ",'[1]Complete Route Listing'!D45)</f>
-        <v>#REF!</v>
+      <c r="C207" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D167=0," ",'[1]Complete Route Listing'!D167)</f>
+        <v>8a+</v>
       </c>
       <c r="D207" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F167=0," ",'[1]Complete Route Listing'!F167)</f>
@@ -7402,9 +7399,9 @@
         <f>IF('[1]Complete Route Listing'!C168=0," ",'[1]Complete Route Listing'!C168)</f>
         <v>black</v>
       </c>
-      <c r="C208" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D48=0," ",'[1]Complete Route Listing'!D48)</f>
-        <v>#REF!</v>
+      <c r="C208" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D168=0," ",'[1]Complete Route Listing'!D168)</f>
+        <v>6b+</v>
       </c>
       <c r="D208" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F168=0," ",'[1]Complete Route Listing'!F168)</f>
@@ -7426,7 +7423,7 @@
         <v>#REF!</v>
       </c>
       <c r="C209" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D49=0," ",'[1]Complete Route Listing'!D49)</f>
+        <f>IF('[1]Complete Route Listing'!D169=0," ",'[1]Complete Route Listing'!D169)</f>
         <v>#REF!</v>
       </c>
       <c r="D209" s="13" t="e">
@@ -7448,9 +7445,9 @@
         <f>IF('[1]Complete Route Listing'!C170=0," ",'[1]Complete Route Listing'!C170)</f>
         <v>pink</v>
       </c>
-      <c r="C210" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D52=0," ",'[1]Complete Route Listing'!D52)</f>
-        <v>#REF!</v>
+      <c r="C210" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D170=0," ",'[1]Complete Route Listing'!D170)</f>
+        <v>7b+</v>
       </c>
       <c r="D210" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F170=0," ",'[1]Complete Route Listing'!F170)</f>
@@ -7471,9 +7468,9 @@
         <f>IF('[1]Complete Route Listing'!C171=0," ",'[1]Complete Route Listing'!C171)</f>
         <v>flo yellow</v>
       </c>
-      <c r="C211" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D53=0," ",'[1]Complete Route Listing'!D53)</f>
-        <v>#REF!</v>
+      <c r="C211" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D171=0," ",'[1]Complete Route Listing'!D171)</f>
+        <v>7a</v>
       </c>
       <c r="D211" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F171=0," ",'[1]Complete Route Listing'!F171)</f>
@@ -7494,9 +7491,9 @@
         <f>IF('[1]Complete Route Listing'!C172=0," ",'[1]Complete Route Listing'!C172)</f>
         <v>blue</v>
       </c>
-      <c r="C212" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D56=0," ",'[1]Complete Route Listing'!D56)</f>
-        <v>#REF!</v>
+      <c r="C212" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D172=0," ",'[1]Complete Route Listing'!D172)</f>
+        <v>6a</v>
       </c>
       <c r="D212" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F172=0," ",'[1]Complete Route Listing'!F172)</f>
@@ -7518,7 +7515,7 @@
         <v>#REF!</v>
       </c>
       <c r="C213" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D57=0," ",'[1]Complete Route Listing'!D57)</f>
+        <f>IF('[1]Complete Route Listing'!D173=0," ",'[1]Complete Route Listing'!D173)</f>
         <v>#REF!</v>
       </c>
       <c r="D213" s="13" t="e">
@@ -7540,9 +7537,9 @@
         <f>IF('[1]Complete Route Listing'!C174=0," ",'[1]Complete Route Listing'!C174)</f>
         <v>white</v>
       </c>
-      <c r="C214" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D109=0," ",'[1]Complete Route Listing'!D109)</f>
-        <v>#REF!</v>
+      <c r="C214" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D174=0," ",'[1]Complete Route Listing'!D174)</f>
+        <v>7a</v>
       </c>
       <c r="D214" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F174=0," ",'[1]Complete Route Listing'!F174)</f>
@@ -7563,9 +7560,9 @@
         <f>IF('[1]Complete Route Listing'!C175=0," ",'[1]Complete Route Listing'!C175)</f>
         <v>yellow</v>
       </c>
-      <c r="C215" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D112=0," ",'[1]Complete Route Listing'!D112)</f>
-        <v>#REF!</v>
+      <c r="C215" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D175=0," ",'[1]Complete Route Listing'!D175)</f>
+        <v>6b</v>
       </c>
       <c r="D215" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F175=0," ",'[1]Complete Route Listing'!F175)</f>
@@ -7586,9 +7583,9 @@
         <f>IF('[1]Complete Route Listing'!C176=0," ",'[1]Complete Route Listing'!C176)</f>
         <v>orange</v>
       </c>
-      <c r="C216" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D113=0," ",'[1]Complete Route Listing'!D113)</f>
-        <v>#REF!</v>
+      <c r="C216" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D176=0," ",'[1]Complete Route Listing'!D176)</f>
+        <v>6b</v>
       </c>
       <c r="D216" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F176=0," ",'[1]Complete Route Listing'!F176)</f>
@@ -7609,9 +7606,9 @@
         <f>IF('[1]Complete Route Listing'!C177=0," ",'[1]Complete Route Listing'!C177)</f>
         <v>red</v>
       </c>
-      <c r="C217" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D116=0," ",'[1]Complete Route Listing'!D116)</f>
-        <v>#REF!</v>
+      <c r="C217" s="12">
+        <f>IF('[1]Complete Route Listing'!D177=0," ",'[1]Complete Route Listing'!D177)</f>
+        <v>5</v>
       </c>
       <c r="D217" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F177=0," ",'[1]Complete Route Listing'!F177)</f>
@@ -7632,9 +7629,9 @@
         <f>IF('[1]Complete Route Listing'!C177=0," ",'[1]Complete Route Listing'!C177)</f>
         <v>red</v>
       </c>
-      <c r="C218" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D117=0," ",'[1]Complete Route Listing'!D117)</f>
-        <v>#REF!</v>
+      <c r="C218" s="12">
+        <f>IF('[1]Complete Route Listing'!D177=0," ",'[1]Complete Route Listing'!D177)</f>
+        <v>5</v>
       </c>
       <c r="D218" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F177=0," ",'[1]Complete Route Listing'!F177)</f>
@@ -7655,9 +7652,9 @@
         <f>IF('[1]Complete Route Listing'!C178=0," ",'[1]Complete Route Listing'!C178)</f>
         <v>green</v>
       </c>
-      <c r="C219" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D121=0," ",'[1]Complete Route Listing'!D121)</f>
-        <v>#REF!</v>
+      <c r="C219" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D178=0," ",'[1]Complete Route Listing'!D178)</f>
+        <v>5+</v>
       </c>
       <c r="D219" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F178=0," ",'[1]Complete Route Listing'!F178)</f>
@@ -7678,9 +7675,9 @@
         <f>IF('[1]Complete Route Listing'!C179=0," ",'[1]Complete Route Listing'!C179)</f>
         <v>white</v>
       </c>
-      <c r="C220" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D124=0," ",'[1]Complete Route Listing'!D124)</f>
-        <v>#REF!</v>
+      <c r="C220" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D179=0," ",'[1]Complete Route Listing'!D179)</f>
+        <v>6c+</v>
       </c>
       <c r="D220" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F179=0," ",'[1]Complete Route Listing'!F179)</f>
@@ -7702,7 +7699,7 @@
         <v>#REF!</v>
       </c>
       <c r="C221" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D125=0," ",'[1]Complete Route Listing'!D125)</f>
+        <f>IF('[1]Complete Route Listing'!D181=0," ",'[1]Complete Route Listing'!D181)</f>
         <v>#REF!</v>
       </c>
       <c r="D221" s="13" t="e">
@@ -7724,9 +7721,9 @@
         <f>IF('[1]Complete Route Listing'!C182=0," ",'[1]Complete Route Listing'!C182)</f>
         <v>blue</v>
       </c>
-      <c r="C222" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D129=0," ",'[1]Complete Route Listing'!D129)</f>
-        <v>#REF!</v>
+      <c r="C222" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D182=0," ",'[1]Complete Route Listing'!D182)</f>
+        <v>6b+</v>
       </c>
       <c r="D222" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F182=0," ",'[1]Complete Route Listing'!F182)</f>
@@ -7747,9 +7744,9 @@
         <f>IF('[1]Complete Route Listing'!C183=0," ",'[1]Complete Route Listing'!C183)</f>
         <v>yellow</v>
       </c>
-      <c r="C223" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D133=0," ",'[1]Complete Route Listing'!D133)</f>
-        <v>#REF!</v>
+      <c r="C223" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D183=0," ",'[1]Complete Route Listing'!D183)</f>
+        <v>5+</v>
       </c>
       <c r="D223" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F183=0," ",'[1]Complete Route Listing'!F183)</f>
@@ -7771,7 +7768,7 @@
         <v>#REF!</v>
       </c>
       <c r="C224" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D136=0," ",'[1]Complete Route Listing'!D136)</f>
+        <f>IF('[1]Complete Route Listing'!D184=0," ",'[1]Complete Route Listing'!D184)</f>
         <v>#REF!</v>
       </c>
       <c r="D224" s="13" t="str">
@@ -7794,7 +7791,7 @@
         <v>#REF!</v>
       </c>
       <c r="C225" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D137=0," ",'[1]Complete Route Listing'!D137)</f>
+        <f>IF('[1]Complete Route Listing'!D185=0," ",'[1]Complete Route Listing'!D185)</f>
         <v>#REF!</v>
       </c>
       <c r="D225" s="13" t="e">
@@ -7816,9 +7813,9 @@
         <f>IF('[1]Complete Route Listing'!C186=0," ",'[1]Complete Route Listing'!C186)</f>
         <v>white</v>
       </c>
-      <c r="C226" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D140=0," ",'[1]Complete Route Listing'!D140)</f>
-        <v>#REF!</v>
+      <c r="C226" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D186=0," ",'[1]Complete Route Listing'!D186)</f>
+        <v>6a</v>
       </c>
       <c r="D226" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F186=0," ",'[1]Complete Route Listing'!F186)</f>
@@ -7839,9 +7836,9 @@
         <f>IF('[1]Complete Route Listing'!C187=0," ",'[1]Complete Route Listing'!C187)</f>
         <v>pink</v>
       </c>
-      <c r="C227" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D141=0," ",'[1]Complete Route Listing'!D141)</f>
-        <v>#REF!</v>
+      <c r="C227" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D187=0," ",'[1]Complete Route Listing'!D187)</f>
+        <v>6a+</v>
       </c>
       <c r="D227" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F187=0," ",'[1]Complete Route Listing'!F187)</f>
@@ -7863,7 +7860,7 @@
         <v>#REF!</v>
       </c>
       <c r="C228" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D145=0," ",'[1]Complete Route Listing'!D145)</f>
+        <f>IF('[1]Complete Route Listing'!D188=0," ",'[1]Complete Route Listing'!D188)</f>
         <v>#REF!</v>
       </c>
       <c r="D228" s="13" t="str">
@@ -7886,7 +7883,7 @@
         <v>#REF!</v>
       </c>
       <c r="C229" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D149=0," ",'[1]Complete Route Listing'!D149)</f>
+        <f>IF('[1]Complete Route Listing'!D189=0," ",'[1]Complete Route Listing'!D189)</f>
         <v>#REF!</v>
       </c>
       <c r="D229" s="13" t="e">
@@ -7908,9 +7905,9 @@
         <f>IF('[1]Complete Route Listing'!C190=0," ",'[1]Complete Route Listing'!C190)</f>
         <v>yellow</v>
       </c>
-      <c r="C230" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D153=0," ",'[1]Complete Route Listing'!D153)</f>
-        <v>#REF!</v>
+      <c r="C230" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D190=0," ",'[1]Complete Route Listing'!D190)</f>
+        <v>6c+</v>
       </c>
       <c r="D230" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F190=0," ",'[1]Complete Route Listing'!F190)</f>
@@ -7931,9 +7928,9 @@
         <f>IF('[1]Complete Route Listing'!C191=0," ",'[1]Complete Route Listing'!C191)</f>
         <v>black</v>
       </c>
-      <c r="C231" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D202=0," ",'[1]Complete Route Listing'!D202)</f>
-        <v>#REF!</v>
+      <c r="C231" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D191=0," ",'[1]Complete Route Listing'!D191)</f>
+        <v>7a+</v>
       </c>
       <c r="D231" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F191=0," ",'[1]Complete Route Listing'!F191)</f>
@@ -7954,9 +7951,9 @@
         <f>IF('[1]Complete Route Listing'!C192=0," ",'[1]Complete Route Listing'!C192)</f>
         <v>green</v>
       </c>
-      <c r="C232" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D203=0," ",'[1]Complete Route Listing'!D203)</f>
-        <v>#REF!</v>
+      <c r="C232" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D192=0," ",'[1]Complete Route Listing'!D192)</f>
+        <v>6a</v>
       </c>
       <c r="D232" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F192=0," ",'[1]Complete Route Listing'!F192)</f>
@@ -7978,7 +7975,7 @@
         <v>#REF!</v>
       </c>
       <c r="C233" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D204=0," ",'[1]Complete Route Listing'!D204)</f>
+        <f>IF('[1]Complete Route Listing'!D193=0," ",'[1]Complete Route Listing'!D193)</f>
         <v>#REF!</v>
       </c>
       <c r="D233" s="13" t="str">
@@ -8000,9 +7997,9 @@
         <f>IF('[1]Complete Route Listing'!C194=0," ",'[1]Complete Route Listing'!C194)</f>
         <v>white</v>
       </c>
-      <c r="C234" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D205=0," ",'[1]Complete Route Listing'!D205)</f>
-        <v>#REF!</v>
+      <c r="C234" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D194=0," ",'[1]Complete Route Listing'!D194)</f>
+        <v>6b+</v>
       </c>
       <c r="D234" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F194=0," ",'[1]Complete Route Listing'!F194)</f>
@@ -8023,9 +8020,9 @@
         <f>IF('[1]Complete Route Listing'!C195=0," ",'[1]Complete Route Listing'!C195)</f>
         <v>flo yellow</v>
       </c>
-      <c r="C235" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D213=0," ",'[1]Complete Route Listing'!D213)</f>
-        <v>#REF!</v>
+      <c r="C235" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D195=0," ",'[1]Complete Route Listing'!D195)</f>
+        <v>6a</v>
       </c>
       <c r="D235" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F195=0," ",'[1]Complete Route Listing'!F195)</f>
@@ -8046,9 +8043,9 @@
         <f>IF('[1]Complete Route Listing'!C196=0," ",'[1]Complete Route Listing'!C196)</f>
         <v>purple</v>
       </c>
-      <c r="C236" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D217=0," ",'[1]Complete Route Listing'!D217)</f>
-        <v>#REF!</v>
+      <c r="C236" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D196=0," ",'[1]Complete Route Listing'!D196)</f>
+        <v>6a+</v>
       </c>
       <c r="D236" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F196=0," ",'[1]Complete Route Listing'!F196)</f>
@@ -8070,7 +8067,7 @@
         <v>#REF!</v>
       </c>
       <c r="C237" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D221=0," ",'[1]Complete Route Listing'!D221)</f>
+        <f>IF('[1]Complete Route Listing'!D197=0," ",'[1]Complete Route Listing'!D197)</f>
         <v>#REF!</v>
       </c>
       <c r="D237" s="13" t="str">
@@ -8092,9 +8089,9 @@
         <f>IF('[1]Complete Route Listing'!C198=0," ",'[1]Complete Route Listing'!C198)</f>
         <v>green</v>
       </c>
-      <c r="C238" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D225=0," ",'[1]Complete Route Listing'!D225)</f>
-        <v>#REF!</v>
+      <c r="C238" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D198=0," ",'[1]Complete Route Listing'!D198)</f>
+        <v>6a</v>
       </c>
       <c r="D238" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F198=0," ",'[1]Complete Route Listing'!F198)</f>
@@ -8115,9 +8112,9 @@
         <f>IF('[1]Complete Route Listing'!C199=0," ",'[1]Complete Route Listing'!C199)</f>
         <v>blue</v>
       </c>
-      <c r="C239" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D229=0," ",'[1]Complete Route Listing'!D229)</f>
-        <v>#REF!</v>
+      <c r="C239" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D199=0," ",'[1]Complete Route Listing'!D199)</f>
+        <v>6b</v>
       </c>
       <c r="D239" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F199=0," ",'[1]Complete Route Listing'!F199)</f>
@@ -8138,9 +8135,9 @@
         <f>IF('[1]Complete Route Listing'!C200=0," ",'[1]Complete Route Listing'!C200)</f>
         <v>orange</v>
       </c>
-      <c r="C240" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D231=0," ",'[1]Complete Route Listing'!D231)</f>
-        <v>#REF!</v>
+      <c r="C240" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D200=0," ",'[1]Complete Route Listing'!D200)</f>
+        <v>6c</v>
       </c>
       <c r="D240" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F200=0," ",'[1]Complete Route Listing'!F200)</f>
@@ -8161,9 +8158,9 @@
         <f>IF('[1]Complete Route Listing'!C201=0," ",'[1]Complete Route Listing'!C201)</f>
         <v>red</v>
       </c>
-      <c r="C241" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D232=0," ",'[1]Complete Route Listing'!D232)</f>
-        <v>#REF!</v>
+      <c r="C241" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D201=0," ",'[1]Complete Route Listing'!D201)</f>
+        <v>6a+</v>
       </c>
       <c r="D241" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F201=0," ",'[1]Complete Route Listing'!F201)</f>
@@ -8178,10 +8175,7 @@
     <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="10"/>
       <c r="B242" s="13"/>
-      <c r="C242" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D233=0," ",'[1]Complete Route Listing'!D233)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="C242" s="12"/>
       <c r="D242" s="13"/>
       <c r="E242" s="11"/>
       <c r="F242" s="14"/>
@@ -8198,9 +8192,9 @@
         <f>IF('[1]Complete Route Listing'!C254=0," ",'[1]Complete Route Listing'!C254)</f>
         <v>red</v>
       </c>
-      <c r="C243" s="7" t="e">
-        <f>IF('[1]Complete Route Listing'!D236=0," ",'[1]Complete Route Listing'!D236)</f>
-        <v>#REF!</v>
+      <c r="C243" s="7" t="str">
+        <f>IF('[1]Complete Route Listing'!D254=0," ",'[1]Complete Route Listing'!D254)</f>
+        <v>6c</v>
       </c>
       <c r="D243" s="8" t="str">
         <f>IF('[1]Complete Route Listing'!F254=0," ",'[1]Complete Route Listing'!F254)</f>
@@ -8221,9 +8215,9 @@
         <f>IF('[1]Complete Route Listing'!C255=0," ",'[1]Complete Route Listing'!C255)</f>
         <v>purple</v>
       </c>
-      <c r="C244" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D237=0," ",'[1]Complete Route Listing'!D237)</f>
-        <v>#REF!</v>
+      <c r="C244" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D255=0," ",'[1]Complete Route Listing'!D255)</f>
+        <v>6c+</v>
       </c>
       <c r="D244" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F255=0," ",'[1]Complete Route Listing'!F255)</f>
@@ -8244,9 +8238,9 @@
         <f>IF('[1]Complete Route Listing'!C256=0," ",'[1]Complete Route Listing'!C256)</f>
         <v>pink</v>
       </c>
-      <c r="C245" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D244=0," ",'[1]Complete Route Listing'!D244)</f>
-        <v>#REF!</v>
+      <c r="C245" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D256=0," ",'[1]Complete Route Listing'!D256)</f>
+        <v>6a+</v>
       </c>
       <c r="D245" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F256=0," ",'[1]Complete Route Listing'!F256)</f>
@@ -8267,9 +8261,9 @@
         <f>IF('[1]Complete Route Listing'!C257=0," ",'[1]Complete Route Listing'!C257)</f>
         <v>blue</v>
       </c>
-      <c r="C246" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D245=0," ",'[1]Complete Route Listing'!D245)</f>
-        <v>#REF!</v>
+      <c r="C246" s="12">
+        <f>IF('[1]Complete Route Listing'!D257=0," ",'[1]Complete Route Listing'!D257)</f>
+        <v>4</v>
       </c>
       <c r="D246" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F257=0," ",'[1]Complete Route Listing'!F257)</f>
@@ -8290,9 +8284,9 @@
         <f>IF('[1]Complete Route Listing'!C257=0," ",'[1]Complete Route Listing'!C257)</f>
         <v>blue</v>
       </c>
-      <c r="C247" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D249=0," ",'[1]Complete Route Listing'!D249)</f>
-        <v>#REF!</v>
+      <c r="C247" s="12">
+        <f>IF('[1]Complete Route Listing'!D257=0," ",'[1]Complete Route Listing'!D257)</f>
+        <v>4</v>
       </c>
       <c r="D247" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F257=0," ",'[1]Complete Route Listing'!F257)</f>
@@ -8313,9 +8307,9 @@
         <f>IF('[1]Complete Route Listing'!C258=0," ",'[1]Complete Route Listing'!C258)</f>
         <v>white</v>
       </c>
-      <c r="C248" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D252=0," ",'[1]Complete Route Listing'!D252)</f>
-        <v>#REF!</v>
+      <c r="C248" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D258=0," ",'[1]Complete Route Listing'!D258)</f>
+        <v>6a+</v>
       </c>
       <c r="D248" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F258=0," ",'[1]Complete Route Listing'!F258)</f>
@@ -8336,9 +8330,9 @@
         <f>IF('[1]Complete Route Listing'!C259=0," ",'[1]Complete Route Listing'!C259)</f>
         <v>yellow</v>
       </c>
-      <c r="C249" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D60=0," ",'[1]Complete Route Listing'!D60)</f>
-        <v>#REF!</v>
+      <c r="C249" s="12">
+        <f>IF('[1]Complete Route Listing'!D259=0," ",'[1]Complete Route Listing'!D259)</f>
+        <v>5</v>
       </c>
       <c r="D249" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F259=0," ",'[1]Complete Route Listing'!F259)</f>
@@ -8360,7 +8354,7 @@
         <v>#REF!</v>
       </c>
       <c r="C250" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D61=0," ",'[1]Complete Route Listing'!D61)</f>
+        <f>IF('[1]Complete Route Listing'!D261=0," ",'[1]Complete Route Listing'!D261)</f>
         <v>#REF!</v>
       </c>
       <c r="D250" s="13" t="e">
@@ -8382,9 +8376,9 @@
         <f>IF('[1]Complete Route Listing'!C262=0," ",'[1]Complete Route Listing'!C262)</f>
         <v>green</v>
       </c>
-      <c r="C251" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D64=0," ",'[1]Complete Route Listing'!D64)</f>
-        <v>#REF!</v>
+      <c r="C251" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D262=0," ",'[1]Complete Route Listing'!D262)</f>
+        <v>6b</v>
       </c>
       <c r="D251" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F262=0," ",'[1]Complete Route Listing'!F262)</f>
@@ -8405,9 +8399,9 @@
         <f>IF('[1]Complete Route Listing'!C263=0," ",'[1]Complete Route Listing'!C263)</f>
         <v>orange</v>
       </c>
-      <c r="C252" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D65=0," ",'[1]Complete Route Listing'!D65)</f>
-        <v>#REF!</v>
+      <c r="C252" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D263=0," ",'[1]Complete Route Listing'!D263)</f>
+        <v>6c</v>
       </c>
       <c r="D252" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F263=0," ",'[1]Complete Route Listing'!F263)</f>
@@ -8428,9 +8422,9 @@
         <f>IF('[1]Complete Route Listing'!C264=0," ",'[1]Complete Route Listing'!C264)</f>
         <v>pink</v>
       </c>
-      <c r="C253" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D68=0," ",'[1]Complete Route Listing'!D68)</f>
-        <v>#REF!</v>
+      <c r="C253" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D264=0," ",'[1]Complete Route Listing'!D264)</f>
+        <v>5+</v>
       </c>
       <c r="D253" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F264=0," ",'[1]Complete Route Listing'!F264)</f>
@@ -8452,7 +8446,7 @@
         <v>#REF!</v>
       </c>
       <c r="C254" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D69=0," ",'[1]Complete Route Listing'!D69)</f>
+        <f>IF('[1]Complete Route Listing'!D265=0," ",'[1]Complete Route Listing'!D265)</f>
         <v>#REF!</v>
       </c>
       <c r="D254" s="13" t="e">
@@ -8474,9 +8468,9 @@
         <f>IF('[1]Complete Route Listing'!C266=0," ",'[1]Complete Route Listing'!C266)</f>
         <v>red</v>
       </c>
-      <c r="C255" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D73=0," ",'[1]Complete Route Listing'!D73)</f>
-        <v>#REF!</v>
+      <c r="C255" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D266=0," ",'[1]Complete Route Listing'!D266)</f>
+        <v>6b</v>
       </c>
       <c r="D255" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F266=0," ",'[1]Complete Route Listing'!F266)</f>
@@ -8497,9 +8491,9 @@
         <f>IF('[1]Complete Route Listing'!C267=0," ",'[1]Complete Route Listing'!C267)</f>
         <v>blue</v>
       </c>
-      <c r="C256" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D77=0," ",'[1]Complete Route Listing'!D77)</f>
-        <v>#REF!</v>
+      <c r="C256" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D267=0," ",'[1]Complete Route Listing'!D267)</f>
+        <v>6b</v>
       </c>
       <c r="D256" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F267=0," ",'[1]Complete Route Listing'!F267)</f>
@@ -8520,9 +8514,9 @@
         <f>IF('[1]Complete Route Listing'!C268=0," ",'[1]Complete Route Listing'!C268)</f>
         <v>purple</v>
       </c>
-      <c r="C257" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D81=0," ",'[1]Complete Route Listing'!D81)</f>
-        <v>#REF!</v>
+      <c r="C257" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D268=0," ",'[1]Complete Route Listing'!D268)</f>
+        <v>4+</v>
       </c>
       <c r="D257" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F268=0," ",'[1]Complete Route Listing'!F268)</f>
@@ -8544,7 +8538,7 @@
         <v>#REF!</v>
       </c>
       <c r="C258" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D89=0," ",'[1]Complete Route Listing'!D89)</f>
+        <f>IF('[1]Complete Route Listing'!D269=0," ",'[1]Complete Route Listing'!D269)</f>
         <v>#REF!</v>
       </c>
       <c r="D258" s="13" t="e">
@@ -8566,9 +8560,9 @@
         <f>IF('[1]Complete Route Listing'!C270=0," ",'[1]Complete Route Listing'!C270)</f>
         <v>orange</v>
       </c>
-      <c r="C259" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D93=0," ",'[1]Complete Route Listing'!D93)</f>
-        <v>#REF!</v>
+      <c r="C259" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D270=0," ",'[1]Complete Route Listing'!D270)</f>
+        <v>6a+</v>
       </c>
       <c r="D259" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F270=0," ",'[1]Complete Route Listing'!F270)</f>
@@ -8586,9 +8580,9 @@
         <f>IF('[1]Complete Route Listing'!C271=0," ",'[1]Complete Route Listing'!C271)</f>
         <v>yellow</v>
       </c>
-      <c r="C260" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D97=0," ",'[1]Complete Route Listing'!D97)</f>
-        <v>#REF!</v>
+      <c r="C260" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D271=0," ",'[1]Complete Route Listing'!D271)</f>
+        <v>6c+</v>
       </c>
       <c r="D260" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F271=0," ",'[1]Complete Route Listing'!F271)</f>
@@ -8606,9 +8600,9 @@
         <f>IF('[1]Complete Route Listing'!C272=0," ",'[1]Complete Route Listing'!C272)</f>
         <v>pink</v>
       </c>
-      <c r="C261" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D105=0," ",'[1]Complete Route Listing'!D105)</f>
-        <v>#REF!</v>
+      <c r="C261" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D272=0," ",'[1]Complete Route Listing'!D272)</f>
+        <v>4+</v>
       </c>
       <c r="D261" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F272=0," ",'[1]Complete Route Listing'!F272)</f>
@@ -8627,7 +8621,7 @@
         <v>#REF!</v>
       </c>
       <c r="C262" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D156=0," ",'[1]Complete Route Listing'!D156)</f>
+        <f>IF('[1]Complete Route Listing'!D273=0," ",'[1]Complete Route Listing'!D273)</f>
         <v>#REF!</v>
       </c>
       <c r="D262" s="13" t="e">
@@ -8646,9 +8640,9 @@
         <f>IF('[1]Complete Route Listing'!C274=0," ",'[1]Complete Route Listing'!C274)</f>
         <v>red</v>
       </c>
-      <c r="C263" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D157=0," ",'[1]Complete Route Listing'!D157)</f>
-        <v>#REF!</v>
+      <c r="C263" s="12">
+        <f>IF('[1]Complete Route Listing'!D274=0," ",'[1]Complete Route Listing'!D274)</f>
+        <v>4</v>
       </c>
       <c r="D263" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F274=0," ",'[1]Complete Route Listing'!F274)</f>
@@ -8666,9 +8660,9 @@
         <f>IF('[1]Complete Route Listing'!C275=0," ",'[1]Complete Route Listing'!C275)</f>
         <v>white</v>
       </c>
-      <c r="C264" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D161=0," ",'[1]Complete Route Listing'!D161)</f>
-        <v>#REF!</v>
+      <c r="C264" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D275=0," ",'[1]Complete Route Listing'!D275)</f>
+        <v>6a</v>
       </c>
       <c r="D264" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F275=0," ",'[1]Complete Route Listing'!F275)</f>
@@ -8686,9 +8680,9 @@
         <f>IF('[1]Complete Route Listing'!C276=0," ",'[1]Complete Route Listing'!C276)</f>
         <v>green</v>
       </c>
-      <c r="C265" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D165=0," ",'[1]Complete Route Listing'!D165)</f>
-        <v>#REF!</v>
+      <c r="C265" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D276=0," ",'[1]Complete Route Listing'!D276)</f>
+        <v>6a</v>
       </c>
       <c r="D265" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F276=0," ",'[1]Complete Route Listing'!F276)</f>
@@ -8707,7 +8701,7 @@
         <v>#REF!</v>
       </c>
       <c r="C266" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D169=0," ",'[1]Complete Route Listing'!D169)</f>
+        <f>IF('[1]Complete Route Listing'!D277=0," ",'[1]Complete Route Listing'!D277)</f>
         <v>#REF!</v>
       </c>
       <c r="D266" s="13" t="e">
@@ -8726,9 +8720,9 @@
         <f>IF('[1]Complete Route Listing'!C278=0," ",'[1]Complete Route Listing'!C278)</f>
         <v>blue</v>
       </c>
-      <c r="C267" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D173=0," ",'[1]Complete Route Listing'!D173)</f>
-        <v>#REF!</v>
+      <c r="C267" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D278=0," ",'[1]Complete Route Listing'!D278)</f>
+        <v>6a</v>
       </c>
       <c r="D267" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F278=0," ",'[1]Complete Route Listing'!F278)</f>
@@ -8746,9 +8740,9 @@
         <f>IF('[1]Complete Route Listing'!C279=0," ",'[1]Complete Route Listing'!C279)</f>
         <v>purple</v>
       </c>
-      <c r="C268" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D181=0," ",'[1]Complete Route Listing'!D181)</f>
-        <v>#REF!</v>
+      <c r="C268" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D279=0," ",'[1]Complete Route Listing'!D279)</f>
+        <v>6c</v>
       </c>
       <c r="D268" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F279=0," ",'[1]Complete Route Listing'!F279)</f>
@@ -8766,9 +8760,9 @@
         <f>IF('[1]Complete Route Listing'!C280=0," ",'[1]Complete Route Listing'!C280)</f>
         <v>pink</v>
       </c>
-      <c r="C269" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D184=0," ",'[1]Complete Route Listing'!D184)</f>
-        <v>#REF!</v>
+      <c r="C269" s="12">
+        <f>IF('[1]Complete Route Listing'!D280=0," ",'[1]Complete Route Listing'!D280)</f>
+        <v>4</v>
       </c>
       <c r="D269" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F280=0," ",'[1]Complete Route Listing'!F280)</f>
@@ -8787,7 +8781,7 @@
         <v>#REF!</v>
       </c>
       <c r="C270" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D185=0," ",'[1]Complete Route Listing'!D185)</f>
+        <f>IF('[1]Complete Route Listing'!D281=0," ",'[1]Complete Route Listing'!D281)</f>
         <v>#REF!</v>
       </c>
       <c r="D270" s="13" t="e">
@@ -8806,9 +8800,9 @@
         <f>IF('[1]Complete Route Listing'!C282=0," ",'[1]Complete Route Listing'!C282)</f>
         <v>black</v>
       </c>
-      <c r="C271" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D188=0," ",'[1]Complete Route Listing'!D188)</f>
-        <v>#REF!</v>
+      <c r="C271" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D282=0," ",'[1]Complete Route Listing'!D282)</f>
+        <v>4+</v>
       </c>
       <c r="D271" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F282=0," ",'[1]Complete Route Listing'!F282)</f>
@@ -8826,9 +8820,9 @@
         <f>IF('[1]Complete Route Listing'!C283=0," ",'[1]Complete Route Listing'!C283)</f>
         <v>orange</v>
       </c>
-      <c r="C272" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D189=0," ",'[1]Complete Route Listing'!D189)</f>
-        <v>#REF!</v>
+      <c r="C272" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D283=0," ",'[1]Complete Route Listing'!D283)</f>
+        <v>6a</v>
       </c>
       <c r="D272" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F283=0," ",'[1]Complete Route Listing'!F283)</f>
@@ -8847,7 +8841,7 @@
         <v>#REF!</v>
       </c>
       <c r="C273" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D193=0," ",'[1]Complete Route Listing'!D193)</f>
+        <f>IF('[1]Complete Route Listing'!D284=0," ",'[1]Complete Route Listing'!D284)</f>
         <v>#REF!</v>
       </c>
       <c r="D273" s="13" t="str">
@@ -8867,7 +8861,7 @@
         <v>#REF!</v>
       </c>
       <c r="C274" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D197=0," ",'[1]Complete Route Listing'!D197)</f>
+        <f>IF('[1]Complete Route Listing'!D285=0," ",'[1]Complete Route Listing'!D285)</f>
         <v>#REF!</v>
       </c>
       <c r="D274" s="13" t="e">
@@ -8886,9 +8880,9 @@
         <f>IF('[1]Complete Route Listing'!C286=0," ",'[1]Complete Route Listing'!C286)</f>
         <v>green</v>
       </c>
-      <c r="C275" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D261=0," ",'[1]Complete Route Listing'!D261)</f>
-        <v>#REF!</v>
+      <c r="C275" s="12">
+        <f>IF('[1]Complete Route Listing'!D286=0," ",'[1]Complete Route Listing'!D286)</f>
+        <v>5</v>
       </c>
       <c r="D275" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F286=0," ",'[1]Complete Route Listing'!F286)</f>
@@ -8906,9 +8900,9 @@
         <f>IF('[1]Complete Route Listing'!C287=0," ",'[1]Complete Route Listing'!C287)</f>
         <v>flo yellow</v>
       </c>
-      <c r="C276" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D265=0," ",'[1]Complete Route Listing'!D265)</f>
-        <v>#REF!</v>
+      <c r="C276" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D287=0," ",'[1]Complete Route Listing'!D287)</f>
+        <v>6b</v>
       </c>
       <c r="D276" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F287=0," ",'[1]Complete Route Listing'!F287)</f>
@@ -8926,9 +8920,9 @@
         <f>IF('[1]Complete Route Listing'!C288=0," ",'[1]Complete Route Listing'!C288)</f>
         <v>purple</v>
       </c>
-      <c r="C277" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D269=0," ",'[1]Complete Route Listing'!D269)</f>
-        <v>#REF!</v>
+      <c r="C277" s="12">
+        <f>IF('[1]Complete Route Listing'!D288=0," ",'[1]Complete Route Listing'!D288)</f>
+        <v>4</v>
       </c>
       <c r="D277" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F288=0," ",'[1]Complete Route Listing'!F288)</f>
@@ -8947,7 +8941,7 @@
         <v>#REF!</v>
       </c>
       <c r="C278" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D273=0," ",'[1]Complete Route Listing'!D273)</f>
+        <f>IF('[1]Complete Route Listing'!D289=0," ",'[1]Complete Route Listing'!D289)</f>
         <v>#REF!</v>
       </c>
       <c r="D278" s="13" t="e">
@@ -8966,9 +8960,9 @@
         <f>IF('[1]Complete Route Listing'!C290=0," ",'[1]Complete Route Listing'!C290)</f>
         <v>pink</v>
       </c>
-      <c r="C279" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D277=0," ",'[1]Complete Route Listing'!D277)</f>
-        <v>#REF!</v>
+      <c r="C279" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D290=0," ",'[1]Complete Route Listing'!D290)</f>
+        <v>5+</v>
       </c>
       <c r="D279" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F290=0," ",'[1]Complete Route Listing'!F290)</f>
@@ -8986,9 +8980,9 @@
         <f>IF('[1]Complete Route Listing'!C291=0," ",'[1]Complete Route Listing'!C291)</f>
         <v>white</v>
       </c>
-      <c r="C280" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D281=0," ",'[1]Complete Route Listing'!D281)</f>
-        <v>#REF!</v>
+      <c r="C280" s="12">
+        <f>IF('[1]Complete Route Listing'!D291=0," ",'[1]Complete Route Listing'!D291)</f>
+        <v>4</v>
       </c>
       <c r="D280" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F291=0," ",'[1]Complete Route Listing'!F291)</f>
@@ -9007,7 +9001,7 @@
         <v>#REF!</v>
       </c>
       <c r="C281" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D284=0," ",'[1]Complete Route Listing'!D284)</f>
+        <f>IF('[1]Complete Route Listing'!D292=0," ",'[1]Complete Route Listing'!D292)</f>
         <v>#REF!</v>
       </c>
       <c r="D281" s="13" t="str">
@@ -9027,7 +9021,7 @@
         <v>#REF!</v>
       </c>
       <c r="C282" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D285=0," ",'[1]Complete Route Listing'!D285)</f>
+        <f>IF('[1]Complete Route Listing'!D293=0," ",'[1]Complete Route Listing'!D293)</f>
         <v>#REF!</v>
       </c>
       <c r="D282" s="13" t="e">
@@ -9046,9 +9040,9 @@
         <f>IF('[1]Complete Route Listing'!C294=0," ",'[1]Complete Route Listing'!C294)</f>
         <v>red</v>
       </c>
-      <c r="C283" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D289=0," ",'[1]Complete Route Listing'!D289)</f>
-        <v>#REF!</v>
+      <c r="C283" s="12" t="str">
+        <f>IF('[1]Complete Route Listing'!D294=0," ",'[1]Complete Route Listing'!D294)</f>
+        <v>6b</v>
       </c>
       <c r="D283" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F294=0," ",'[1]Complete Route Listing'!F294)</f>
@@ -9066,9 +9060,9 @@
         <f>IF('[1]Complete Route Listing'!C295=0," ",'[1]Complete Route Listing'!C295)</f>
         <v>black</v>
       </c>
-      <c r="C284" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D292=0," ",'[1]Complete Route Listing'!D292)</f>
-        <v>#REF!</v>
+      <c r="C284" s="12">
+        <f>IF('[1]Complete Route Listing'!D295=0," ",'[1]Complete Route Listing'!D295)</f>
+        <v>5</v>
       </c>
       <c r="D284" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F295=0," ",'[1]Complete Route Listing'!F295)</f>
@@ -9087,7 +9081,7 @@
         <v>#REF!</v>
       </c>
       <c r="C285" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D293=0," ",'[1]Complete Route Listing'!D293)</f>
+        <f>IF('[1]Complete Route Listing'!D296=0," ",'[1]Complete Route Listing'!D296)</f>
         <v>#REF!</v>
       </c>
       <c r="D285" s="13" t="str">
@@ -9107,7 +9101,7 @@
         <v>#REF!</v>
       </c>
       <c r="C286" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D296=0," ",'[1]Complete Route Listing'!D296)</f>
+        <f>IF('[1]Complete Route Listing'!D297=0," ",'[1]Complete Route Listing'!D297)</f>
         <v>#REF!</v>
       </c>
       <c r="D286" s="13" t="e">
@@ -9126,9 +9120,9 @@
         <f>IF('[1]Complete Route Listing'!C298=0," ",'[1]Complete Route Listing'!C298)</f>
         <v>white</v>
       </c>
-      <c r="C287" s="12" t="e">
-        <f>IF('[1]Complete Route Listing'!D297=0," ",'[1]Complete Route Listing'!D297)</f>
-        <v>#REF!</v>
+      <c r="C287" s="12">
+        <f>IF('[1]Complete Route Listing'!D298=0," ",'[1]Complete Route Listing'!D298)</f>
+        <v>3</v>
       </c>
       <c r="D287" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F298=0," ",'[1]Complete Route Listing'!F298)</f>
@@ -9146,7 +9140,10 @@
         <f>IF('[1]Complete Route Listing'!C299=0," ",'[1]Complete Route Listing'!C299)</f>
         <v>green</v>
       </c>
-      <c r="C288" s="12"/>
+      <c r="C288" s="12">
+        <f>IF('[1]Complete Route Listing'!D299=0," ",'[1]Complete Route Listing'!D299)</f>
+        <v>4</v>
+      </c>
       <c r="D288" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F299=0," ",'[1]Complete Route Listing'!F299)</f>
         <v>OCT</v>
@@ -9163,7 +9160,10 @@
         <f>IF('[1]Complete Route Listing'!C300=0," ",'[1]Complete Route Listing'!C300)</f>
         <v>blue</v>
       </c>
-      <c r="C289" s="12"/>
+      <c r="C289" s="12">
+        <f>IF('[1]Complete Route Listing'!D300=0," ",'[1]Complete Route Listing'!D300)</f>
+        <v>3</v>
+      </c>
       <c r="D289" s="13" t="str">
         <f>IF('[1]Complete Route Listing'!F300=0," ",'[1]Complete Route Listing'!F300)</f>
         <v>OCT</v>
@@ -9172,9 +9172,6 @@
       <c r="F289" s="14"/>
     </row>
   </sheetData>
-  <sortState ref="C2:C289">
-    <sortCondition ref="C1"/>
-  </sortState>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.94488188976377963" bottom="0.94488188976377963" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>